<commit_message>
Update published master datasets (2026-02-18)
</commit_message>
<xml_diff>
--- a/archive/InnovateUK_Funding_Opportunities_Latest_2026-02-18.xlsx
+++ b/archive/InnovateUK_Funding_Opportunities_Latest_2026-02-18.xlsx
@@ -1262,7 +1262,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1340,6 +1340,62 @@
         <is>
           <t>Week commencing (Wed)</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Innovate UK Business Connect</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Southwest Wales Net Zero Industry Launchpad Round 2 - Call for challenge holders</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://iuk-business-connect.org.uk/opportunities/southwest-wales-net-zero-industry-launchpad-round-2-call-for-challenge-holders/</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2026-02-18 10:32</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>46071.43888888889</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>18/02/2026</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>46071</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>13/03/2026                              00:00</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>46094</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>£25,000</t>
+        </is>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>46071</v>
       </c>
     </row>
   </sheetData>
@@ -1353,7 +1409,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1385,189 +1441,189 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46064</v>
+        <v>46071</v>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46057</v>
+        <v>46064</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46050</v>
+        <v>46057</v>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46043</v>
+        <v>46050</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>46036</v>
+        <v>46043</v>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D6" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>46029</v>
+        <v>46036</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D7" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>46022</v>
+        <v>46029</v>
       </c>
       <c r="B8" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D8" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>46015</v>
+        <v>46022</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C9" t="n">
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>46008</v>
+        <v>46015</v>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>46001</v>
+        <v>46008</v>
       </c>
       <c r="B11" t="n">
         <v>2</v>
       </c>
       <c r="C11" t="n">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="D11" t="n">
-        <v>79</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45994</v>
+        <v>46001</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45987</v>
+        <v>45994</v>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45980</v>
+        <v>45987</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45973</v>
+        <v>45980</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
@@ -1581,91 +1637,91 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45966</v>
+        <v>45973</v>
       </c>
       <c r="B16" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45959</v>
+        <v>45966</v>
       </c>
       <c r="B17" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45952</v>
+        <v>45959</v>
       </c>
       <c r="B18" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45945</v>
+        <v>45952</v>
       </c>
       <c r="B19" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45938</v>
+        <v>45945</v>
       </c>
       <c r="B20" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45931</v>
+        <v>45938</v>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45924</v>
+        <v>45931</v>
       </c>
       <c r="B22" t="n">
         <v>1</v>
@@ -1679,35 +1735,35 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45917</v>
+        <v>45924</v>
       </c>
       <c r="B23" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45910</v>
+        <v>45917</v>
       </c>
       <c r="B24" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45903</v>
+        <v>45910</v>
       </c>
       <c r="B25" t="n">
         <v>2</v>
@@ -1721,169 +1777,183 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45896</v>
+        <v>45903</v>
       </c>
       <c r="B26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45889</v>
+        <v>45896</v>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45882</v>
+        <v>45889</v>
       </c>
       <c r="B28" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45875</v>
+        <v>45882</v>
       </c>
       <c r="B29" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45868</v>
+        <v>45875</v>
       </c>
       <c r="B30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45861</v>
+        <v>45868</v>
       </c>
       <c r="B31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45854</v>
+        <v>45861</v>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45847</v>
+        <v>45854</v>
       </c>
       <c r="B33" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45840</v>
+        <v>45847</v>
       </c>
       <c r="B34" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45833</v>
+        <v>45840</v>
       </c>
       <c r="B35" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45826</v>
+        <v>45833</v>
       </c>
       <c r="B36" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
+        <v>45826</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
         <v>45819</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B38" t="n">
         <v>25</v>
       </c>
-      <c r="C37" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" t="n">
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1898,7 +1968,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N250"/>
+  <dimension ref="A1:N251"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9253,26 +9323,26 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Innovate Funding Service</t>
+          <t>Innovate UK Business Connect</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Future Leaders Fellowships: Round 10, business and non-academic</t>
+          <t>Southwest Wales Net Zero Industry Launchpad Round 2 - Call for challenge holders</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2058/overview/0f904547-f415-4fb9-94a7-0701c38a2ba1</t>
+          <t>https://iuk-business-connect.org.uk/opportunities/southwest-wales-net-zero-industry-launchpad-round-2-call-for-challenge-holders/</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>2025-06-14 08:41</t>
+          <t>2026-02-18 10:32</t>
         </is>
       </c>
       <c r="E147" s="1" t="n">
-        <v>45822.36180555556</v>
+        <v>46071.43888888889</v>
       </c>
       <c r="F147" t="b">
         <v>1</v>
@@ -9281,23 +9351,29 @@
       <c r="H147" t="b">
         <v>0</v>
       </c>
-      <c r="I147" t="inlineStr"/>
-      <c r="J147" t="inlineStr"/>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>18/02/2026</t>
+        </is>
+      </c>
+      <c r="J147" s="1" t="n">
+        <v>46071</v>
+      </c>
       <c r="K147" t="inlineStr">
         <is>
-          <t>Wednesday 5 November 2025 11:00am</t>
+          <t>13/03/2026                              00:00</t>
         </is>
       </c>
       <c r="L147" s="1" t="n">
-        <v>45966.45833333334</v>
+        <v>46094</v>
       </c>
       <c r="M147" t="inlineStr">
         <is>
-          <t>£3.0 million</t>
+          <t>£25,000</t>
         </is>
       </c>
       <c r="N147" s="1" t="n">
-        <v>45819</v>
+        <v>46071</v>
       </c>
     </row>
     <row r="148">
@@ -9308,12 +9384,12 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>ADOPT Facilitator Support Grant: Round 2</t>
+          <t>Future Leaders Fellowships: Round 10, business and non-academic</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2223/overview/4e423e05-3228-45e3-9cfe-0b39d1227307</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2058/overview/0f904547-f415-4fb9-94a7-0701c38a2ba1</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -9335,15 +9411,15 @@
       <c r="J148" t="inlineStr"/>
       <c r="K148" t="inlineStr">
         <is>
-          <t>Thursday 24 July 2025 11:00am</t>
+          <t>Wednesday 5 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L148" s="1" t="n">
-        <v>45862.45833333334</v>
+        <v>45966.45833333334</v>
       </c>
       <c r="M148" t="inlineStr">
         <is>
-          <t>£2,500</t>
+          <t>£3.0 million</t>
         </is>
       </c>
       <c r="N148" s="1" t="n">
@@ -9358,12 +9434,12 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>MSI Improving energy or resource efficiency in manufacturing FS</t>
+          <t>ADOPT Facilitator Support Grant: Round 2</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2225/overview/c43ef163-3872-4178-b80d-88c406691610</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2223/overview/4e423e05-3228-45e3-9cfe-0b39d1227307</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -9385,15 +9461,15 @@
       <c r="J149" t="inlineStr"/>
       <c r="K149" t="inlineStr">
         <is>
-          <t>Wednesday 2 July 2025 11:00am</t>
+          <t>Thursday 24 July 2025 11:00am</t>
         </is>
       </c>
       <c r="L149" s="1" t="n">
-        <v>45840.45833333334</v>
+        <v>45862.45833333334</v>
       </c>
       <c r="M149" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£2,500</t>
         </is>
       </c>
       <c r="N149" s="1" t="n">
@@ -9408,12 +9484,12 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>New Innovators in Marine and Maritime, Great South West</t>
+          <t>MSI Improving energy or resource efficiency in manufacturing FS</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2215/overview/67b86d6c-bab9-4a01-aacc-3da2e57edc99</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2225/overview/c43ef163-3872-4178-b80d-88c406691610</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -9443,7 +9519,7 @@
       </c>
       <c r="M150" t="inlineStr">
         <is>
-          <t>£50,000</t>
+          <t>£100,000</t>
         </is>
       </c>
       <c r="N150" s="1" t="n">
@@ -9458,12 +9534,12 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Commercialising Knowledge Assets Fund (CKAF) Autumn</t>
+          <t>New Innovators in Marine and Maritime, Great South West</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2217/overview/c555f64e-5485-4e49-89b8-32d61fac4ff0</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2215/overview/67b86d6c-bab9-4a01-aacc-3da2e57edc99</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -9485,15 +9561,15 @@
       <c r="J151" t="inlineStr"/>
       <c r="K151" t="inlineStr">
         <is>
-          <t>Thursday 4 September 2025 11:00am</t>
+          <t>Wednesday 2 July 2025 11:00am</t>
         </is>
       </c>
       <c r="L151" s="1" t="n">
-        <v>45904.45833333334</v>
+        <v>45840.45833333334</v>
       </c>
       <c r="M151" t="inlineStr">
         <is>
-          <t>£250,000</t>
+          <t>£50,000</t>
         </is>
       </c>
       <c r="N151" s="1" t="n">
@@ -9508,12 +9584,12 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>ATI Programme strategic batch: EoI – June 2025</t>
+          <t>Commercialising Knowledge Assets Fund (CKAF) Autumn</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2218/overview/a45dcc8a-b621-4a79-9e4d-046e19b6b1e9</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2217/overview/c555f64e-5485-4e49-89b8-32d61fac4ff0</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -9535,13 +9611,17 @@
       <c r="J152" t="inlineStr"/>
       <c r="K152" t="inlineStr">
         <is>
-          <t>Wednesday 18 June 2025 11:00am</t>
+          <t>Thursday 4 September 2025 11:00am</t>
         </is>
       </c>
       <c r="L152" s="1" t="n">
-        <v>45826.45833333334</v>
-      </c>
-      <c r="M152" t="inlineStr"/>
+        <v>45904.45833333334</v>
+      </c>
+      <c r="M152" t="inlineStr">
+        <is>
+          <t>£250,000</t>
+        </is>
+      </c>
       <c r="N152" s="1" t="n">
         <v>45819</v>
       </c>
@@ -9554,12 +9634,12 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Defra Farming Innovation Investor Partnership</t>
+          <t>ATI Programme strategic batch: EoI – June 2025</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2207/overview/05e5263b-75a1-49a0-87f0-261541af0840</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2218/overview/a45dcc8a-b621-4a79-9e4d-046e19b6b1e9</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -9581,17 +9661,13 @@
       <c r="J153" t="inlineStr"/>
       <c r="K153" t="inlineStr">
         <is>
-          <t>Wednesday 2 July 2025 11:00am</t>
+          <t>Wednesday 18 June 2025 11:00am</t>
         </is>
       </c>
       <c r="L153" s="1" t="n">
-        <v>45840.45833333334</v>
-      </c>
-      <c r="M153" t="inlineStr">
-        <is>
-          <t>£3.0 million</t>
-        </is>
-      </c>
+        <v>45826.45833333334</v>
+      </c>
+      <c r="M153" t="inlineStr"/>
       <c r="N153" s="1" t="n">
         <v>45819</v>
       </c>
@@ -9604,12 +9680,12 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Ofgem Strategic Innovation Fund Round 5 Discovery C3</t>
+          <t>Defra Farming Innovation Investor Partnership</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2204/overview/9da241b9-1fd8-49fb-b8d0-4a81a637b3b5</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2207/overview/05e5263b-75a1-49a0-87f0-261541af0840</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -9631,15 +9707,15 @@
       <c r="J154" t="inlineStr"/>
       <c r="K154" t="inlineStr">
         <is>
-          <t>Wednesday 25 June 2025 11:00am</t>
+          <t>Wednesday 2 July 2025 11:00am</t>
         </is>
       </c>
       <c r="L154" s="1" t="n">
-        <v>45833.45833333334</v>
+        <v>45840.45833333334</v>
       </c>
       <c r="M154" t="inlineStr">
         <is>
-          <t>£150,000</t>
+          <t>£3.0 million</t>
         </is>
       </c>
       <c r="N154" s="1" t="n">
@@ -9654,12 +9730,12 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Ofgem Strategic Innovation Fund Round 4 Discovery C3</t>
+          <t>Ofgem Strategic Innovation Fund Round 5 Discovery C3</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2200/overview/0f0721c8-5a37-4046-8e4f-7649194e8adc</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2204/overview/9da241b9-1fd8-49fb-b8d0-4a81a637b3b5</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -9704,12 +9780,12 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: Scaling community initiatives in diet and exercise</t>
+          <t>Ofgem Strategic Innovation Fund Round 4 Discovery C3</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2191/overview/6a097cf8-8f81-495d-b56f-3f240cfde64c</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2200/overview/0f0721c8-5a37-4046-8e4f-7649194e8adc</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -9731,15 +9807,15 @@
       <c r="J156" t="inlineStr"/>
       <c r="K156" t="inlineStr">
         <is>
-          <t>Wednesday 18 June 2025 11:00am</t>
+          <t>Wednesday 25 June 2025 11:00am</t>
         </is>
       </c>
       <c r="L156" s="1" t="n">
-        <v>45826.45833333334</v>
+        <v>45833.45833333334</v>
       </c>
       <c r="M156" t="inlineStr">
         <is>
-          <t>£250,000</t>
+          <t>£150,000</t>
         </is>
       </c>
       <c r="N156" s="1" t="n">
@@ -9754,12 +9830,12 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: Quantum Sensors and PNT Missions Primer</t>
+          <t>Contracts for Innovation: Scaling community initiatives in diet and exercise</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2209/overview/28f8801b-a8b3-48c8-8c81-64d75341b81d</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2191/overview/6a097cf8-8f81-495d-b56f-3f240cfde64c</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -9781,15 +9857,15 @@
       <c r="J157" t="inlineStr"/>
       <c r="K157" t="inlineStr">
         <is>
-          <t>Wednesday 2 July 2025 11:00am</t>
+          <t>Wednesday 18 June 2025 11:00am</t>
         </is>
       </c>
       <c r="L157" s="1" t="n">
-        <v>45840.45833333334</v>
+        <v>45826.45833333334</v>
       </c>
       <c r="M157" t="inlineStr">
         <is>
-          <t>£1.5 million</t>
+          <t>£250,000</t>
         </is>
       </c>
       <c r="N157" s="1" t="n">
@@ -9804,12 +9880,12 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: Net Zero Living Tech Trials, phase 3</t>
+          <t>Contracts for Innovation: Quantum Sensors and PNT Missions Primer</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2189/overview/a59ac38e-662b-49a5-b7f9-a44c2cc38c61</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2209/overview/28f8801b-a8b3-48c8-8c81-64d75341b81d</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -9831,15 +9907,15 @@
       <c r="J158" t="inlineStr"/>
       <c r="K158" t="inlineStr">
         <is>
-          <t>Wednesday 25 June 2025 11:00am</t>
+          <t>Wednesday 2 July 2025 11:00am</t>
         </is>
       </c>
       <c r="L158" s="1" t="n">
-        <v>45833.45833333334</v>
+        <v>45840.45833333334</v>
       </c>
       <c r="M158" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£1.5 million</t>
         </is>
       </c>
       <c r="N158" s="1" t="n">
@@ -9854,12 +9930,12 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: Clean Air, Phase 3</t>
+          <t>Contracts for Innovation: Net Zero Living Tech Trials, phase 3</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2181/overview/02aad9d2-c984-4bd5-a3f6-80f25ec62870</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2189/overview/a59ac38e-662b-49a5-b7f9-a44c2cc38c61</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -9904,12 +9980,12 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: DSbD Advancing CHERI Tools and software</t>
+          <t>Contracts for Innovation: Clean Air, Phase 3</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2194/overview/91c68630-20eb-4247-8296-ae1737637756</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2181/overview/02aad9d2-c984-4bd5-a3f6-80f25ec62870</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -9931,15 +10007,15 @@
       <c r="J160" t="inlineStr"/>
       <c r="K160" t="inlineStr">
         <is>
-          <t>Wednesday 18 June 2025 11:00am</t>
+          <t>Wednesday 25 June 2025 11:00am</t>
         </is>
       </c>
       <c r="L160" s="1" t="n">
-        <v>45826.45833333334</v>
+        <v>45833.45833333334</v>
       </c>
       <c r="M160" t="inlineStr">
         <is>
-          <t>£3.0 million</t>
+          <t>£100,000</t>
         </is>
       </c>
       <c r="N160" s="1" t="n">
@@ -9954,12 +10030,12 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: DSbD Advancing CHERI RISC-V Devices</t>
+          <t>Contracts for Innovation: DSbD Advancing CHERI Tools and software</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2198/overview/b2e2fd41-d372-4e33-a6df-8bfefb8de0f9</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2194/overview/91c68630-20eb-4247-8296-ae1737637756</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -9989,7 +10065,7 @@
       </c>
       <c r="M161" t="inlineStr">
         <is>
-          <t>£5.0 million</t>
+          <t>£3.0 million</t>
         </is>
       </c>
       <c r="N161" s="1" t="n">
@@ -10004,12 +10080,12 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Canada-UK Semiconductors</t>
+          <t>Contracts for Innovation: DSbD Advancing CHERI RISC-V Devices</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2192/overview/3906cbd5-fec2-4c1f-897d-ccab071708b3</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2198/overview/b2e2fd41-d372-4e33-a6df-8bfefb8de0f9</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
@@ -10031,15 +10107,15 @@
       <c r="J162" t="inlineStr"/>
       <c r="K162" t="inlineStr">
         <is>
-          <t>Wednesday 15 October 2025 11:00am</t>
+          <t>Wednesday 18 June 2025 11:00am</t>
         </is>
       </c>
       <c r="L162" s="1" t="n">
-        <v>45945.45833333334</v>
+        <v>45826.45833333334</v>
       </c>
       <c r="M162" t="inlineStr">
         <is>
-          <t>£500,000</t>
+          <t>£5.0 million</t>
         </is>
       </c>
       <c r="N162" s="1" t="n">
@@ -10054,12 +10130,12 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Accelerated Knowledge Transfer 4 (AKT4) Addiction</t>
+          <t>Canada-UK Semiconductors</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2178/overview/2699060f-dd6f-415b-ae47-bead15aa430e</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2192/overview/3906cbd5-fec2-4c1f-897d-ccab071708b3</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
@@ -10081,15 +10157,15 @@
       <c r="J163" t="inlineStr"/>
       <c r="K163" t="inlineStr">
         <is>
-          <t>Wednesday 2 July 2025 11:00am</t>
+          <t>Wednesday 15 October 2025 11:00am</t>
         </is>
       </c>
       <c r="L163" s="1" t="n">
-        <v>45840.45833333334</v>
+        <v>45945.45833333334</v>
       </c>
       <c r="M163" t="inlineStr">
         <is>
-          <t>£35,000</t>
+          <t>£500,000</t>
         </is>
       </c>
       <c r="N163" s="1" t="n">
@@ -10104,12 +10180,12 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Innovate UK innovation loans future economy: Round 21</t>
+          <t>Accelerated Knowledge Transfer 4 (AKT4) Addiction</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2188/overview/20c89a26-2479-4f80-b35a-b62ed3b9b3ce</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2178/overview/2699060f-dd6f-415b-ae47-bead15aa430e</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
@@ -10139,7 +10215,7 @@
       </c>
       <c r="M164" t="inlineStr">
         <is>
-          <t>£2.0 million</t>
+          <t>£35,000</t>
         </is>
       </c>
       <c r="N164" s="1" t="n">
@@ -10154,12 +10230,12 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Farming Futures R&amp;D Fund: Precision Breeding Competition</t>
+          <t>Innovate UK innovation loans future economy: Round 21</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2168/overview/0fef9171-75b0-4f3e-acef-42920e7e5d5e</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2188/overview/20c89a26-2479-4f80-b35a-b62ed3b9b3ce</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
@@ -10181,15 +10257,15 @@
       <c r="J165" t="inlineStr"/>
       <c r="K165" t="inlineStr">
         <is>
-          <t>Wednesday 25 June 2025 11:00am</t>
+          <t>Wednesday 2 July 2025 11:00am</t>
         </is>
       </c>
       <c r="L165" s="1" t="n">
-        <v>45833.45833333334</v>
+        <v>45840.45833333334</v>
       </c>
       <c r="M165" t="inlineStr">
         <is>
-          <t>£2.5 million</t>
+          <t>£2.0 million</t>
         </is>
       </c>
       <c r="N165" s="1" t="n">
@@ -10204,12 +10280,12 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Farming Futures R&amp;D Fund: low emissions farming</t>
+          <t>Farming Futures R&amp;D Fund: Precision Breeding Competition</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2169/overview/64b0d550-3f46-4ab4-a0cd-5fa7ac488cb6</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2168/overview/0fef9171-75b0-4f3e-acef-42920e7e5d5e</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
@@ -10254,12 +10330,12 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Investor Partnerships: Clean Energy and Climate Technologies</t>
+          <t>Farming Futures R&amp;D Fund: low emissions farming</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2175/overview/7487b4f1-51e6-4f15-a4c8-f103559d14bb</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2169/overview/64b0d550-3f46-4ab4-a0cd-5fa7ac488cb6</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
@@ -10281,15 +10357,15 @@
       <c r="J167" t="inlineStr"/>
       <c r="K167" t="inlineStr">
         <is>
-          <t>Wednesday 2 July 2025 11:00am</t>
+          <t>Wednesday 25 June 2025 11:00am</t>
         </is>
       </c>
       <c r="L167" s="1" t="n">
-        <v>45840.45833333334</v>
+        <v>45833.45833333334</v>
       </c>
       <c r="M167" t="inlineStr">
         <is>
-          <t>£2.0 million</t>
+          <t>£2.5 million</t>
         </is>
       </c>
       <c r="N167" s="1" t="n">
@@ -10304,12 +10380,12 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Full ADOPT Grant: Round 1</t>
+          <t>Investor Partnerships: Clean Energy and Climate Technologies</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2162/overview/c35de0a9-5072-4142-8a52-1cdce8ef3871</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2175/overview/7487b4f1-51e6-4f15-a4c8-f103559d14bb</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
@@ -10331,15 +10407,15 @@
       <c r="J168" t="inlineStr"/>
       <c r="K168" t="inlineStr">
         <is>
-          <t>Wednesday 25 June 2025 11:00am</t>
+          <t>Wednesday 2 July 2025 11:00am</t>
         </is>
       </c>
       <c r="L168" s="1" t="n">
-        <v>45833.45833333334</v>
+        <v>45840.45833333334</v>
       </c>
       <c r="M168" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£2.0 million</t>
         </is>
       </c>
       <c r="N168" s="1" t="n">
@@ -10354,12 +10430,12 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Horizon Europe Guarantee - EIT KICs 2023</t>
+          <t>Full ADOPT Grant: Round 1</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/1585/overview/32135a71-171a-46bf-ad56-e2e65a1a3574</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2162/overview/c35de0a9-5072-4142-8a52-1cdce8ef3871</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
@@ -10381,11 +10457,17 @@
       <c r="J169" t="inlineStr"/>
       <c r="K169" t="inlineStr">
         <is>
-          <t>Thursday 27 November 2025 4:00pm</t>
-        </is>
-      </c>
-      <c r="L169" t="inlineStr"/>
-      <c r="M169" t="inlineStr"/>
+          <t>Wednesday 25 June 2025 11:00am</t>
+        </is>
+      </c>
+      <c r="L169" s="1" t="n">
+        <v>45833.45833333334</v>
+      </c>
+      <c r="M169" t="inlineStr">
+        <is>
+          <t>£100,000</t>
+        </is>
+      </c>
       <c r="N169" s="1" t="n">
         <v>45819</v>
       </c>
@@ -10398,12 +10480,12 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Horizon Europe Guarantee Extension</t>
+          <t>Horizon Europe Guarantee - EIT KICs 2023</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/1389/overview/b900fdc4-c48d-4d8a-8733-ce4ca210ae9a</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/1585/overview/32135a71-171a-46bf-ad56-e2e65a1a3574</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
@@ -10442,21 +10524,21 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Knowledge Transfer Partnership (KTP): 2025 – 2026 Round 3</t>
+          <t>Horizon Europe Guarantee Extension</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2184/overview/c599b17c-e13a-4e13-995e-53cc4d4508a1</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/1389/overview/b900fdc4-c48d-4d8a-8733-ce4ca210ae9a</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>2025-06-16 22:04</t>
+          <t>2025-06-14 08:41</t>
         </is>
       </c>
       <c r="E171" s="1" t="n">
-        <v>45824.91944444444</v>
+        <v>45822.36180555556</v>
       </c>
       <c r="F171" t="b">
         <v>1</v>
@@ -10469,17 +10551,11 @@
       <c r="J171" t="inlineStr"/>
       <c r="K171" t="inlineStr">
         <is>
-          <t>Wednesday 17 September 2025 11:00am</t>
-        </is>
-      </c>
-      <c r="L171" s="1" t="n">
-        <v>45917.45833333334</v>
-      </c>
-      <c r="M171" t="inlineStr">
-        <is>
-          <t>£8,500</t>
-        </is>
-      </c>
+          <t>Thursday 27 November 2025 4:00pm</t>
+        </is>
+      </c>
+      <c r="L171" t="inlineStr"/>
+      <c r="M171" t="inlineStr"/>
       <c r="N171" s="1" t="n">
         <v>45819</v>
       </c>
@@ -10492,21 +10568,21 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Agri-tech and food technology, Mid and North Wales - CRD</t>
+          <t>Knowledge Transfer Partnership (KTP): 2025 – 2026 Round 3</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2212/overview/4411087f-2a92-4aed-b735-d1a813376bec</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2184/overview/c599b17c-e13a-4e13-995e-53cc4d4508a1</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>2025-06-26 08:52</t>
+          <t>2025-06-16 22:04</t>
         </is>
       </c>
       <c r="E172" s="1" t="n">
-        <v>45834.36944444444</v>
+        <v>45824.91944444444</v>
       </c>
       <c r="F172" t="b">
         <v>1</v>
@@ -10519,19 +10595,19 @@
       <c r="J172" t="inlineStr"/>
       <c r="K172" t="inlineStr">
         <is>
-          <t>Wednesday 20 August 2025 11:00am</t>
+          <t>Wednesday 17 September 2025 11:00am</t>
         </is>
       </c>
       <c r="L172" s="1" t="n">
-        <v>45889.45833333334</v>
+        <v>45917.45833333334</v>
       </c>
       <c r="M172" t="inlineStr">
         <is>
-          <t>£500,000</t>
+          <t>£8,500</t>
         </is>
       </c>
       <c r="N172" s="1" t="n">
-        <v>45833</v>
+        <v>45819</v>
       </c>
     </row>
     <row r="173">
@@ -10542,12 +10618,12 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Full ADOPT Grant Round 2</t>
+          <t>Agri-tech and food technology, Mid and North Wales - CRD</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2222/overview/c3d5b2f9-e4d4-4ddc-99a2-589904ac3d42</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2212/overview/4411087f-2a92-4aed-b735-d1a813376bec</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -10577,7 +10653,7 @@
       </c>
       <c r="M173" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£500,000</t>
         </is>
       </c>
       <c r="N173" s="1" t="n">
@@ -10592,21 +10668,21 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Innovate UK Innovation Loans Round 22</t>
+          <t>Full ADOPT Grant Round 2</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2236/overview/70cbae59-4e67-4626-8cb0-6bbbfc0cf6b7</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2222/overview/c3d5b2f9-e4d4-4ddc-99a2-589904ac3d42</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>2025-07-03 08:52</t>
+          <t>2025-06-26 08:52</t>
         </is>
       </c>
       <c r="E174" s="1" t="n">
-        <v>45841.36944444444</v>
+        <v>45834.36944444444</v>
       </c>
       <c r="F174" t="b">
         <v>1</v>
@@ -10619,19 +10695,19 @@
       <c r="J174" t="inlineStr"/>
       <c r="K174" t="inlineStr">
         <is>
-          <t>Wednesday 27 August 2025 11:00am</t>
+          <t>Wednesday 20 August 2025 11:00am</t>
         </is>
       </c>
       <c r="L174" s="1" t="n">
-        <v>45896.45833333334</v>
+        <v>45889.45833333334</v>
       </c>
       <c r="M174" t="inlineStr">
         <is>
-          <t>£5.0 million</t>
+          <t>£100,000</t>
         </is>
       </c>
       <c r="N174" s="1" t="n">
-        <v>45840</v>
+        <v>45833</v>
       </c>
     </row>
     <row r="175">
@@ -10642,21 +10718,21 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Growth Catalyst Early Stage: New Innovators</t>
+          <t>Innovate UK Innovation Loans Round 22</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2220/overview/bcfd2780-f307-4434-be32-46889a239024</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2236/overview/70cbae59-4e67-4626-8cb0-6bbbfc0cf6b7</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>2025-07-07 08:54</t>
+          <t>2025-07-03 08:52</t>
         </is>
       </c>
       <c r="E175" s="1" t="n">
-        <v>45845.37083333333</v>
+        <v>45841.36944444444</v>
       </c>
       <c r="F175" t="b">
         <v>1</v>
@@ -10669,15 +10745,15 @@
       <c r="J175" t="inlineStr"/>
       <c r="K175" t="inlineStr">
         <is>
-          <t>Wednesday 6 August 2025 11:00am</t>
+          <t>Wednesday 27 August 2025 11:00am</t>
         </is>
       </c>
       <c r="L175" s="1" t="n">
-        <v>45875.45833333334</v>
+        <v>45896.45833333334</v>
       </c>
       <c r="M175" t="inlineStr">
         <is>
-          <t>£50,000</t>
+          <t>£5.0 million</t>
         </is>
       </c>
       <c r="N175" s="1" t="n">
@@ -10692,12 +10768,12 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>ATI Programme strategic batch: EoI – July 2025</t>
+          <t>Growth Catalyst Early Stage: New Innovators</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2228/overview/5ccf059d-ae66-4f72-a319-4b12cbd46d1c</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2220/overview/bcfd2780-f307-4434-be32-46889a239024</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
@@ -10719,13 +10795,17 @@
       <c r="J176" t="inlineStr"/>
       <c r="K176" t="inlineStr">
         <is>
-          <t>Wednesday 23 July 2025 11:00am</t>
+          <t>Wednesday 6 August 2025 11:00am</t>
         </is>
       </c>
       <c r="L176" s="1" t="n">
-        <v>45861.45833333334</v>
-      </c>
-      <c r="M176" t="inlineStr"/>
+        <v>45875.45833333334</v>
+      </c>
+      <c r="M176" t="inlineStr">
+        <is>
+          <t>£50,000</t>
+        </is>
+      </c>
       <c r="N176" s="1" t="n">
         <v>45840</v>
       </c>
@@ -10738,21 +10818,21 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: Resource Efficient Construction Impacts</t>
+          <t>ATI Programme strategic batch: EoI – July 2025</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2242/overview/51b1338a-0d60-43de-b062-fe7a48a7d42f</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2228/overview/5ccf059d-ae66-4f72-a319-4b12cbd46d1c</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>2025-07-09 08:54</t>
+          <t>2025-07-07 08:54</t>
         </is>
       </c>
       <c r="E177" s="1" t="n">
-        <v>45847.37083333333</v>
+        <v>45845.37083333333</v>
       </c>
       <c r="F177" t="b">
         <v>1</v>
@@ -10765,19 +10845,15 @@
       <c r="J177" t="inlineStr"/>
       <c r="K177" t="inlineStr">
         <is>
-          <t>Wednesday 27 August 2025 11:00am</t>
+          <t>Wednesday 23 July 2025 11:00am</t>
         </is>
       </c>
       <c r="L177" s="1" t="n">
-        <v>45896.45833333334</v>
-      </c>
-      <c r="M177" t="inlineStr">
-        <is>
-          <t>£300,000</t>
-        </is>
-      </c>
+        <v>45861.45833333334</v>
+      </c>
+      <c r="M177" t="inlineStr"/>
       <c r="N177" s="1" t="n">
-        <v>45847</v>
+        <v>45840</v>
       </c>
     </row>
     <row r="178">
@@ -10788,12 +10864,12 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: Resource Efficient Chemicals Impacts</t>
+          <t>Contracts for Innovation: Resource Efficient Construction Impacts</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2240/overview/10f28eca-01f0-4abf-8e0c-998151fe747b</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2242/overview/51b1338a-0d60-43de-b062-fe7a48a7d42f</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
@@ -10838,12 +10914,12 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: Resource Efficient Automotive Impacts</t>
+          <t>Contracts for Innovation: Resource Efficient Chemicals Impacts</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2241/overview/baec7aff-ca8b-456c-9e4d-d6eb9621a988</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2240/overview/10f28eca-01f0-4abf-8e0c-998151fe747b</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
@@ -10888,12 +10964,12 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Future Flight: Regional Demonstrator 2</t>
+          <t>Contracts for Innovation: Resource Efficient Automotive Impacts</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2239/overview/7c5a9acd-4b31-414a-8e35-20dd1df3a2a1</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2241/overview/baec7aff-ca8b-456c-9e4d-d6eb9621a988</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
@@ -10915,15 +10991,15 @@
       <c r="J180" t="inlineStr"/>
       <c r="K180" t="inlineStr">
         <is>
-          <t>Thursday 17 July 2025 11:00am</t>
+          <t>Wednesday 27 August 2025 11:00am</t>
         </is>
       </c>
       <c r="L180" s="1" t="n">
-        <v>45855.45833333334</v>
+        <v>45896.45833333334</v>
       </c>
       <c r="M180" t="inlineStr">
         <is>
-          <t>£200,000</t>
+          <t>£300,000</t>
         </is>
       </c>
       <c r="N180" s="1" t="n">
@@ -10938,21 +11014,21 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>DRIVE35 Scale-up: Feasibility Studies</t>
+          <t>Future Flight: Regional Demonstrator 2</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2247/overview/53da287a-c141-48d2-a3eb-f854e14c6578</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2239/overview/7c5a9acd-4b31-414a-8e35-20dd1df3a2a1</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>2025-07-15 08:20</t>
+          <t>2025-07-09 08:54</t>
         </is>
       </c>
       <c r="E181" s="1" t="n">
-        <v>45853.34722222222</v>
+        <v>45847.37083333333</v>
       </c>
       <c r="F181" t="b">
         <v>1</v>
@@ -10965,15 +11041,15 @@
       <c r="J181" t="inlineStr"/>
       <c r="K181" t="inlineStr">
         <is>
-          <t>Wednesday 3 September 2025 11:00am</t>
+          <t>Thursday 17 July 2025 11:00am</t>
         </is>
       </c>
       <c r="L181" s="1" t="n">
-        <v>45903.45833333334</v>
+        <v>45855.45833333334</v>
       </c>
       <c r="M181" t="inlineStr">
         <is>
-          <t>£750,000</t>
+          <t>£200,000</t>
         </is>
       </c>
       <c r="N181" s="1" t="n">
@@ -10988,12 +11064,12 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>DRIVE35 Innovation Fund: Demonstrate</t>
+          <t>DRIVE35 Scale-up: Feasibility Studies</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2245/overview/777781a3-f181-42b3-a05e-86b96754f28d</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2247/overview/53da287a-c141-48d2-a3eb-f854e14c6578</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
@@ -11015,15 +11091,15 @@
       <c r="J182" t="inlineStr"/>
       <c r="K182" t="inlineStr">
         <is>
-          <t>Wednesday 1 October 2025 11:00am</t>
+          <t>Wednesday 3 September 2025 11:00am</t>
         </is>
       </c>
       <c r="L182" s="1" t="n">
-        <v>45931.45833333334</v>
+        <v>45903.45833333334</v>
       </c>
       <c r="M182" t="inlineStr">
         <is>
-          <t>£1.5 million</t>
+          <t>£750,000</t>
         </is>
       </c>
       <c r="N182" s="1" t="n">
@@ -11038,12 +11114,12 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>DRIVE35 Innovation Fund: Collaborate</t>
+          <t>DRIVE35 Innovation Fund: Demonstrate</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2244/overview/84f81488-4936-4551-a315-7ec40cf1065d</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2245/overview/777781a3-f181-42b3-a05e-86b96754f28d</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
@@ -11073,7 +11149,7 @@
       </c>
       <c r="M183" t="inlineStr">
         <is>
-          <t>£25.0 million</t>
+          <t>£1.5 million</t>
         </is>
       </c>
       <c r="N183" s="1" t="n">
@@ -11088,21 +11164,21 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>ADOPT Facilitator Support Grant: Round 3</t>
+          <t>DRIVE35 Innovation Fund: Collaborate</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2251/overview/f40e861a-c7f6-4597-ac5d-2e8d1b4f59f8</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2244/overview/84f81488-4936-4551-a315-7ec40cf1065d</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>2025-07-25 08:20</t>
+          <t>2025-07-15 08:20</t>
         </is>
       </c>
       <c r="E184" s="1" t="n">
-        <v>45863.34722222222</v>
+        <v>45853.34722222222</v>
       </c>
       <c r="F184" t="b">
         <v>1</v>
@@ -11115,19 +11191,19 @@
       <c r="J184" t="inlineStr"/>
       <c r="K184" t="inlineStr">
         <is>
-          <t>Wednesday 3 September 2025 11:00am</t>
+          <t>Wednesday 1 October 2025 11:00am</t>
         </is>
       </c>
       <c r="L184" s="1" t="n">
-        <v>45903.45833333334</v>
+        <v>45931.45833333334</v>
       </c>
       <c r="M184" t="inlineStr">
         <is>
-          <t>£2,500</t>
+          <t>£25.0 million</t>
         </is>
       </c>
       <c r="N184" s="1" t="n">
-        <v>45861</v>
+        <v>45847</v>
       </c>
     </row>
     <row r="185">
@@ -11138,21 +11214,21 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Sovereign AI - Proof of concept</t>
+          <t>ADOPT Facilitator Support Grant: Round 3</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2259/overview/9061ddb2-fa12-45c9-8691-d36649c96e9c</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2251/overview/f40e861a-c7f6-4597-ac5d-2e8d1b4f59f8</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>2025-08-07 08:21</t>
+          <t>2025-07-25 08:20</t>
         </is>
       </c>
       <c r="E185" s="1" t="n">
-        <v>45876.34791666667</v>
+        <v>45863.34722222222</v>
       </c>
       <c r="F185" t="b">
         <v>1</v>
@@ -11165,19 +11241,19 @@
       <c r="J185" t="inlineStr"/>
       <c r="K185" t="inlineStr">
         <is>
-          <t>Wednesday 10 September 2025 11:00am</t>
+          <t>Wednesday 3 September 2025 11:00am</t>
         </is>
       </c>
       <c r="L185" s="1" t="n">
-        <v>45910.45833333334</v>
+        <v>45903.45833333334</v>
       </c>
       <c r="M185" t="inlineStr">
         <is>
-          <t>£120,000</t>
+          <t>£2,500</t>
         </is>
       </c>
       <c r="N185" s="1" t="n">
-        <v>45875</v>
+        <v>45861</v>
       </c>
     </row>
     <row r="186">
@@ -11188,21 +11264,21 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Obesity Pathway Innovation Programme (OPIP): Strand 3</t>
+          <t>Sovereign AI - Proof of concept</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2186/overview/e51c18bc-21b3-450d-bdbc-2f43dad3b268</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2259/overview/9061ddb2-fa12-45c9-8691-d36649c96e9c</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>2025-08-14 08:20</t>
+          <t>2025-08-07 08:21</t>
         </is>
       </c>
       <c r="E186" s="1" t="n">
-        <v>45883.34722222222</v>
+        <v>45876.34791666667</v>
       </c>
       <c r="F186" t="b">
         <v>1</v>
@@ -11215,19 +11291,19 @@
       <c r="J186" t="inlineStr"/>
       <c r="K186" t="inlineStr">
         <is>
-          <t>Wednesday 19 November 2025 11:00am</t>
+          <t>Wednesday 10 September 2025 11:00am</t>
         </is>
       </c>
       <c r="L186" s="1" t="n">
-        <v>45980.45833333334</v>
+        <v>45910.45833333334</v>
       </c>
       <c r="M186" t="inlineStr">
         <is>
-          <t>£8.0 million</t>
+          <t>£120,000</t>
         </is>
       </c>
       <c r="N186" s="1" t="n">
-        <v>45882</v>
+        <v>45875</v>
       </c>
     </row>
     <row r="187">
@@ -11238,12 +11314,12 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Obesity Pathway Innovation Programme (OPIP): Strand 2</t>
+          <t>Obesity Pathway Innovation Programme (OPIP): Strand 3</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2185/overview/d5b2aeb3-c2e4-4d78-9be3-f1d9919b0956</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2186/overview/e51c18bc-21b3-450d-bdbc-2f43dad3b268</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
@@ -11273,7 +11349,7 @@
       </c>
       <c r="M187" t="inlineStr">
         <is>
-          <t>£4.5 million</t>
+          <t>£8.0 million</t>
         </is>
       </c>
       <c r="N187" s="1" t="n">
@@ -11288,12 +11364,12 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Obesity Pathway Innovation Programme (OPIP): Strand 1</t>
+          <t>Obesity Pathway Innovation Programme (OPIP): Strand 2</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2177/overview/696c1e3c-589d-4c37-8958-6255d1dc125a</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2185/overview/d5b2aeb3-c2e4-4d78-9be3-f1d9919b0956</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
@@ -11323,7 +11399,7 @@
       </c>
       <c r="M188" t="inlineStr">
         <is>
-          <t>£3.5 million</t>
+          <t>£4.5 million</t>
         </is>
       </c>
       <c r="N188" s="1" t="n">
@@ -11338,21 +11414,21 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Analysis for Innovators: National Physical Laboratory Stage 1</t>
+          <t>Obesity Pathway Innovation Programme (OPIP): Strand 1</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2266/overview/2fcad3ee-b5d6-4f01-8b1a-0e1af3c93023</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2177/overview/696c1e3c-589d-4c37-8958-6255d1dc125a</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>2025-08-26 08:20</t>
+          <t>2025-08-14 08:20</t>
         </is>
       </c>
       <c r="E189" s="1" t="n">
-        <v>45895.34722222222</v>
+        <v>45883.34722222222</v>
       </c>
       <c r="F189" t="b">
         <v>1</v>
@@ -11365,19 +11441,19 @@
       <c r="J189" t="inlineStr"/>
       <c r="K189" t="inlineStr">
         <is>
-          <t>Wednesday 10 September 2025 11:00am</t>
+          <t>Wednesday 19 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L189" s="1" t="n">
-        <v>45910.45833333334</v>
+        <v>45980.45833333334</v>
       </c>
       <c r="M189" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£3.5 million</t>
         </is>
       </c>
       <c r="N189" s="1" t="n">
-        <v>45889</v>
+        <v>45882</v>
       </c>
     </row>
     <row r="190">
@@ -11388,21 +11464,21 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Full ADOPT Grant Round 3</t>
+          <t>Analysis for Innovators: National Physical Laboratory Stage 1</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2265/overview/fae182db-d9e5-4173-bb59-8fde361ccad4</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2266/overview/2fcad3ee-b5d6-4f01-8b1a-0e1af3c93023</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>2025-08-27 08:18</t>
+          <t>2025-08-26 08:20</t>
         </is>
       </c>
       <c r="E190" s="1" t="n">
-        <v>45896.34583333333</v>
+        <v>45895.34722222222</v>
       </c>
       <c r="F190" t="b">
         <v>1</v>
@@ -11415,11 +11491,11 @@
       <c r="J190" t="inlineStr"/>
       <c r="K190" t="inlineStr">
         <is>
-          <t>Wednesday 15 October 2025 11:00am</t>
+          <t>Wednesday 10 September 2025 11:00am</t>
         </is>
       </c>
       <c r="L190" s="1" t="n">
-        <v>45945.45833333334</v>
+        <v>45910.45833333334</v>
       </c>
       <c r="M190" t="inlineStr">
         <is>
@@ -11427,7 +11503,7 @@
         </is>
       </c>
       <c r="N190" s="1" t="n">
-        <v>45896</v>
+        <v>45889</v>
       </c>
     </row>
     <row r="191">
@@ -11438,21 +11514,21 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>ATI Programme strategic batch: EoI – September 2025</t>
+          <t>Full ADOPT Grant Round 3</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2273/overview/b30df196-a9a2-4e53-85e1-e3e6aaa5c5b7</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2265/overview/fae182db-d9e5-4173-bb59-8fde361ccad4</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>2025-09-01 08:20</t>
+          <t>2025-08-27 08:18</t>
         </is>
       </c>
       <c r="E191" s="1" t="n">
-        <v>45901.34722222222</v>
+        <v>45896.34583333333</v>
       </c>
       <c r="F191" t="b">
         <v>1</v>
@@ -11465,13 +11541,17 @@
       <c r="J191" t="inlineStr"/>
       <c r="K191" t="inlineStr">
         <is>
-          <t>Wednesday 17 September 2025 11:00am</t>
+          <t>Wednesday 15 October 2025 11:00am</t>
         </is>
       </c>
       <c r="L191" s="1" t="n">
-        <v>45917.45833333334</v>
-      </c>
-      <c r="M191" t="inlineStr"/>
+        <v>45945.45833333334</v>
+      </c>
+      <c r="M191" t="inlineStr">
+        <is>
+          <t>£100,000</t>
+        </is>
+      </c>
       <c r="N191" s="1" t="n">
         <v>45896</v>
       </c>
@@ -11484,21 +11564,21 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Farming Innovation Programme: Small R&amp;D Partnership Projects Rd 4</t>
+          <t>ATI Programme strategic batch: EoI – September 2025</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2010/overview/bcd5cf06-313c-4197-ae47-0035f674717f</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2273/overview/b30df196-a9a2-4e53-85e1-e3e6aaa5c5b7</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>2025-09-02 08:19</t>
+          <t>2025-09-01 08:20</t>
         </is>
       </c>
       <c r="E192" s="1" t="n">
-        <v>45902.34652777778</v>
+        <v>45901.34722222222</v>
       </c>
       <c r="F192" t="b">
         <v>1</v>
@@ -11511,17 +11591,13 @@
       <c r="J192" t="inlineStr"/>
       <c r="K192" t="inlineStr">
         <is>
-          <t>Wednesday 5 November 2025 11:00am</t>
+          <t>Wednesday 17 September 2025 11:00am</t>
         </is>
       </c>
       <c r="L192" s="1" t="n">
-        <v>45966.45833333334</v>
-      </c>
-      <c r="M192" t="inlineStr">
-        <is>
-          <t>£3.0 million</t>
-        </is>
-      </c>
+        <v>45917.45833333334</v>
+      </c>
+      <c r="M192" t="inlineStr"/>
       <c r="N192" s="1" t="n">
         <v>45896</v>
       </c>
@@ -11534,21 +11610,21 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>ADOPT Facilitator Support Grant: Round 4</t>
+          <t>Farming Innovation Programme: Small R&amp;D Partnership Projects Rd 4</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2277/overview/7386173a-c074-4617-b7d0-f54f3a458247</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2010/overview/bcd5cf06-313c-4197-ae47-0035f674717f</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>2025-09-04 08:18</t>
+          <t>2025-09-02 08:19</t>
         </is>
       </c>
       <c r="E193" s="1" t="n">
-        <v>45904.34583333333</v>
+        <v>45902.34652777778</v>
       </c>
       <c r="F193" t="b">
         <v>1</v>
@@ -11561,19 +11637,19 @@
       <c r="J193" t="inlineStr"/>
       <c r="K193" t="inlineStr">
         <is>
-          <t>Wednesday 15 October 2025 11:00am</t>
+          <t>Wednesday 5 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L193" s="1" t="n">
-        <v>45945.45833333334</v>
+        <v>45966.45833333334</v>
       </c>
       <c r="M193" t="inlineStr">
         <is>
-          <t>£2,500</t>
+          <t>£3.0 million</t>
         </is>
       </c>
       <c r="N193" s="1" t="n">
-        <v>45903</v>
+        <v>45896</v>
       </c>
     </row>
     <row r="194">
@@ -11584,21 +11660,21 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Innovate UK Innovation Loans Round 23</t>
+          <t>ADOPT Facilitator Support Grant: Round 4</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2275/overview/dec9b656-5f30-414e-a169-e11e17d04896</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2277/overview/7386173a-c074-4617-b7d0-f54f3a458247</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>2025-09-05 08:18</t>
+          <t>2025-09-04 08:18</t>
         </is>
       </c>
       <c r="E194" s="1" t="n">
-        <v>45905.34583333333</v>
+        <v>45904.34583333333</v>
       </c>
       <c r="F194" t="b">
         <v>1</v>
@@ -11611,15 +11687,15 @@
       <c r="J194" t="inlineStr"/>
       <c r="K194" t="inlineStr">
         <is>
-          <t>Wednesday 22 October 2025 11:00am</t>
+          <t>Wednesday 15 October 2025 11:00am</t>
         </is>
       </c>
       <c r="L194" s="1" t="n">
-        <v>45952.45833333334</v>
+        <v>45945.45833333334</v>
       </c>
       <c r="M194" t="inlineStr">
         <is>
-          <t>£5.0 million</t>
+          <t>£2,500</t>
         </is>
       </c>
       <c r="N194" s="1" t="n">
@@ -11634,21 +11710,21 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>UK-Netherlands Co-Innovation and Testbeds Pilot for Quantum Tech</t>
+          <t>Innovate UK Innovation Loans Round 23</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2288/overview/d547d84e-d652-4ed6-9c85-b12ab8d785d2</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2275/overview/dec9b656-5f30-414e-a169-e11e17d04896</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>2025-09-12 08:17</t>
+          <t>2025-09-05 08:18</t>
         </is>
       </c>
       <c r="E195" s="1" t="n">
-        <v>45912.34513888889</v>
+        <v>45905.34583333333</v>
       </c>
       <c r="F195" t="b">
         <v>1</v>
@@ -11661,19 +11737,19 @@
       <c r="J195" t="inlineStr"/>
       <c r="K195" t="inlineStr">
         <is>
-          <t>Tuesday 28 October 2025 11:00am</t>
+          <t>Wednesday 22 October 2025 11:00am</t>
         </is>
       </c>
       <c r="L195" s="1" t="n">
-        <v>45958.45833333334</v>
+        <v>45952.45833333334</v>
       </c>
       <c r="M195" t="inlineStr">
         <is>
-          <t>£300,000</t>
+          <t>£5.0 million</t>
         </is>
       </c>
       <c r="N195" s="1" t="n">
-        <v>45910</v>
+        <v>45903</v>
       </c>
     </row>
     <row r="196">
@@ -11684,21 +11760,21 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: Quantum Technologies for Transport - Phase 1</t>
+          <t>UK-Netherlands Co-Innovation and Testbeds Pilot for Quantum Tech</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2292/overview/cdea3182-7495-4cad-8435-f49882f08ec7</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2288/overview/d547d84e-d652-4ed6-9c85-b12ab8d785d2</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>2025-09-16 08:19</t>
+          <t>2025-09-12 08:17</t>
         </is>
       </c>
       <c r="E196" s="1" t="n">
-        <v>45916.34652777778</v>
+        <v>45912.34513888889</v>
       </c>
       <c r="F196" t="b">
         <v>1</v>
@@ -11711,15 +11787,15 @@
       <c r="J196" t="inlineStr"/>
       <c r="K196" t="inlineStr">
         <is>
-          <t>Wednesday 15 October 2025 11:00am</t>
+          <t>Tuesday 28 October 2025 11:00am</t>
         </is>
       </c>
       <c r="L196" s="1" t="n">
-        <v>45945.45833333334</v>
+        <v>45958.45833333334</v>
       </c>
       <c r="M196" t="inlineStr">
         <is>
-          <t>£40,000</t>
+          <t>£300,000</t>
         </is>
       </c>
       <c r="N196" s="1" t="n">
@@ -11734,21 +11810,21 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>DRIVE35 Scale-up Fund</t>
+          <t>Contracts for Innovation: Quantum Technologies for Transport - Phase 1</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2279/overview/029bd996-9abd-42d9-8134-e2d34e3cfff5</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2292/overview/cdea3182-7495-4cad-8435-f49882f08ec7</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>2025-09-17 08:18</t>
+          <t>2025-09-16 08:19</t>
         </is>
       </c>
       <c r="E197" s="1" t="n">
-        <v>45917.34583333333</v>
+        <v>45916.34652777778</v>
       </c>
       <c r="F197" t="b">
         <v>1</v>
@@ -11761,17 +11837,19 @@
       <c r="J197" t="inlineStr"/>
       <c r="K197" t="inlineStr">
         <is>
-          <t>There is no submission deadline</t>
-        </is>
-      </c>
-      <c r="L197" t="inlineStr"/>
+          <t>Wednesday 15 October 2025 11:00am</t>
+        </is>
+      </c>
+      <c r="L197" s="1" t="n">
+        <v>45945.45833333334</v>
+      </c>
       <c r="M197" t="inlineStr">
         <is>
-          <t>£20.0 million</t>
+          <t>£40,000</t>
         </is>
       </c>
       <c r="N197" s="1" t="n">
-        <v>45917</v>
+        <v>45910</v>
       </c>
     </row>
     <row r="198">
@@ -11782,21 +11860,21 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Commercialising Knowledge Assets Fund (CKAF) Winter</t>
+          <t>DRIVE35 Scale-up Fund</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2295/overview/cdce9dab-263c-444b-9e91-61f13046bd62</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2279/overview/029bd996-9abd-42d9-8134-e2d34e3cfff5</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>2025-09-18 08:17</t>
+          <t>2025-09-17 08:18</t>
         </is>
       </c>
       <c r="E198" s="1" t="n">
-        <v>45918.34513888889</v>
+        <v>45917.34583333333</v>
       </c>
       <c r="F198" t="b">
         <v>1</v>
@@ -11809,15 +11887,13 @@
       <c r="J198" t="inlineStr"/>
       <c r="K198" t="inlineStr">
         <is>
-          <t>Thursday 4 December 2025 11:00am</t>
-        </is>
-      </c>
-      <c r="L198" s="1" t="n">
-        <v>45995.45833333334</v>
-      </c>
+          <t>There is no submission deadline</t>
+        </is>
+      </c>
+      <c r="L198" t="inlineStr"/>
       <c r="M198" t="inlineStr">
         <is>
-          <t>£250,000</t>
+          <t>£20.0 million</t>
         </is>
       </c>
       <c r="N198" s="1" t="n">
@@ -11832,21 +11908,21 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Resource efficiency for resilience and sustainability FS</t>
+          <t>Commercialising Knowledge Assets Fund (CKAF) Winter</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2293/overview/2efee934-8622-4686-bc02-a6ac7fc9e5a6</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2295/overview/cdce9dab-263c-444b-9e91-61f13046bd62</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>2025-09-20 08:16</t>
+          <t>2025-09-18 08:17</t>
         </is>
       </c>
       <c r="E199" s="1" t="n">
-        <v>45920.34444444445</v>
+        <v>45918.34513888889</v>
       </c>
       <c r="F199" t="b">
         <v>1</v>
@@ -11859,15 +11935,15 @@
       <c r="J199" t="inlineStr"/>
       <c r="K199" t="inlineStr">
         <is>
-          <t>Monday 3 November 2025 11:00am</t>
+          <t>Thursday 4 December 2025 11:00am</t>
         </is>
       </c>
       <c r="L199" s="1" t="n">
-        <v>45964.45833333334</v>
+        <v>45995.45833333334</v>
       </c>
       <c r="M199" t="inlineStr">
         <is>
-          <t>£25,000</t>
+          <t>£250,000</t>
         </is>
       </c>
       <c r="N199" s="1" t="n">
@@ -11882,21 +11958,21 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Ofgem Strategic Innovation Fund Round 5 Discovery C4</t>
+          <t>Resource efficiency for resilience and sustainability FS</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2284/overview/aa6bd2b1-f6e1-4e96-bd4c-0557c10779c8</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2293/overview/2efee934-8622-4686-bc02-a6ac7fc9e5a6</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>2025-09-23 08:18</t>
+          <t>2025-09-20 08:16</t>
         </is>
       </c>
       <c r="E200" s="1" t="n">
-        <v>45923.34583333333</v>
+        <v>45920.34444444445</v>
       </c>
       <c r="F200" t="b">
         <v>1</v>
@@ -11909,15 +11985,15 @@
       <c r="J200" t="inlineStr"/>
       <c r="K200" t="inlineStr">
         <is>
-          <t>Wednesday 22 October 2025 11:00am</t>
+          <t>Monday 3 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L200" s="1" t="n">
-        <v>45952.45833333334</v>
+        <v>45964.45833333334</v>
       </c>
       <c r="M200" t="inlineStr">
         <is>
-          <t>£150,000</t>
+          <t>£25,000</t>
         </is>
       </c>
       <c r="N200" s="1" t="n">
@@ -11932,21 +12008,21 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Farming Innovation Programme: Feasibility Round 4</t>
+          <t>Ofgem Strategic Innovation Fund Round 5 Discovery C4</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2006/overview/b67973b5-6d46-4a34-a864-bec1212e3fe0</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2284/overview/aa6bd2b1-f6e1-4e96-bd4c-0557c10779c8</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>2025-09-29 08:20</t>
+          <t>2025-09-23 08:18</t>
         </is>
       </c>
       <c r="E201" s="1" t="n">
-        <v>45929.34722222222</v>
+        <v>45923.34583333333</v>
       </c>
       <c r="F201" t="b">
         <v>1</v>
@@ -11959,19 +12035,19 @@
       <c r="J201" t="inlineStr"/>
       <c r="K201" t="inlineStr">
         <is>
-          <t>Wednesday 3 December 2025 11:00am</t>
+          <t>Wednesday 22 October 2025 11:00am</t>
         </is>
       </c>
       <c r="L201" s="1" t="n">
-        <v>45994.45833333334</v>
+        <v>45952.45833333334</v>
       </c>
       <c r="M201" t="inlineStr">
         <is>
-          <t>£500,000</t>
+          <t>£150,000</t>
         </is>
       </c>
       <c r="N201" s="1" t="n">
-        <v>45924</v>
+        <v>45917</v>
       </c>
     </row>
     <row r="202">
@@ -11982,21 +12058,21 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Eureka GlobalStars Japan 2026</t>
+          <t>Farming Innovation Programme: Feasibility Round 4</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2276/overview/19635c62-dd91-41d8-a90e-547cdb5acbfa</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2006/overview/b67973b5-6d46-4a34-a864-bec1212e3fe0</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>2025-10-03 08:17</t>
+          <t>2025-09-29 08:20</t>
         </is>
       </c>
       <c r="E202" s="1" t="n">
-        <v>45933.34513888889</v>
+        <v>45929.34722222222</v>
       </c>
       <c r="F202" t="b">
         <v>1</v>
@@ -12009,19 +12085,19 @@
       <c r="J202" t="inlineStr"/>
       <c r="K202" t="inlineStr">
         <is>
-          <t>Wednesday 21 January 2026 11:00am</t>
+          <t>Wednesday 3 December 2025 11:00am</t>
         </is>
       </c>
       <c r="L202" s="1" t="n">
-        <v>46043.45833333334</v>
+        <v>45994.45833333334</v>
       </c>
       <c r="M202" t="inlineStr">
         <is>
-          <t>£600,000</t>
+          <t>£500,000</t>
         </is>
       </c>
       <c r="N202" s="1" t="n">
-        <v>45931</v>
+        <v>45924</v>
       </c>
     </row>
     <row r="203">
@@ -12032,21 +12108,21 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>CAM Pathfinder: Feasibility studies 2</t>
+          <t>Eureka GlobalStars Japan 2026</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2307/overview/8eec43e7-96a5-49d1-97e1-3400321160f9</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2276/overview/19635c62-dd91-41d8-a90e-547cdb5acbfa</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>2025-10-10 08:18</t>
+          <t>2025-10-03 08:17</t>
         </is>
       </c>
       <c r="E203" s="1" t="n">
-        <v>45940.34583333333</v>
+        <v>45933.34513888889</v>
       </c>
       <c r="F203" t="b">
         <v>1</v>
@@ -12059,19 +12135,19 @@
       <c r="J203" t="inlineStr"/>
       <c r="K203" t="inlineStr">
         <is>
-          <t>Wednesday 26 November 2025 11:00am</t>
+          <t>Wednesday 21 January 2026 11:00am</t>
         </is>
       </c>
       <c r="L203" s="1" t="n">
-        <v>45987.45833333334</v>
+        <v>46043.45833333334</v>
       </c>
       <c r="M203" t="inlineStr">
         <is>
-          <t>£250,000</t>
+          <t>£600,000</t>
         </is>
       </c>
       <c r="N203" s="1" t="n">
-        <v>45938</v>
+        <v>45931</v>
       </c>
     </row>
     <row r="204">
@@ -12082,21 +12158,21 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>ATI Programme strategic batch EoI – October 2025</t>
+          <t>CAM Pathfinder: Feasibility studies 2</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2317/overview/c946fbde-725e-4f85-bb3f-3219576c4a01</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2307/overview/8eec43e7-96a5-49d1-97e1-3400321160f9</t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>2025-10-14 08:17</t>
+          <t>2025-10-10 08:18</t>
         </is>
       </c>
       <c r="E204" s="1" t="n">
-        <v>45944.34513888889</v>
+        <v>45940.34583333333</v>
       </c>
       <c r="F204" t="b">
         <v>1</v>
@@ -12109,13 +12185,17 @@
       <c r="J204" t="inlineStr"/>
       <c r="K204" t="inlineStr">
         <is>
-          <t>Wednesday 22 October 2025 11:00am</t>
+          <t>Wednesday 26 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L204" s="1" t="n">
-        <v>45952.45833333334</v>
-      </c>
-      <c r="M204" t="inlineStr"/>
+        <v>45987.45833333334</v>
+      </c>
+      <c r="M204" t="inlineStr">
+        <is>
+          <t>£250,000</t>
+        </is>
+      </c>
       <c r="N204" s="1" t="n">
         <v>45938</v>
       </c>
@@ -12128,21 +12208,21 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>CAM Pathfinder: Enable</t>
+          <t>ATI Programme strategic batch EoI – October 2025</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2318/overview/39cd0e04-6f9c-40da-b0be-8eaae7f1603d</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2317/overview/c946fbde-725e-4f85-bb3f-3219576c4a01</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>2025-10-15 08:19</t>
+          <t>2025-10-14 08:17</t>
         </is>
       </c>
       <c r="E205" s="1" t="n">
-        <v>45945.34652777778</v>
+        <v>45944.34513888889</v>
       </c>
       <c r="F205" t="b">
         <v>1</v>
@@ -12155,19 +12235,15 @@
       <c r="J205" t="inlineStr"/>
       <c r="K205" t="inlineStr">
         <is>
-          <t>Wednesday 17 December 2025 11:00am</t>
+          <t>Wednesday 22 October 2025 11:00am</t>
         </is>
       </c>
       <c r="L205" s="1" t="n">
-        <v>46008.45833333334</v>
-      </c>
-      <c r="M205" t="inlineStr">
-        <is>
-          <t>£4.0 million</t>
-        </is>
-      </c>
+        <v>45952.45833333334</v>
+      </c>
+      <c r="M205" t="inlineStr"/>
       <c r="N205" s="1" t="n">
-        <v>45945</v>
+        <v>45938</v>
       </c>
     </row>
     <row r="206">
@@ -12178,12 +12254,12 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>CAM Pathfinder: Demonstrate</t>
+          <t>CAM Pathfinder: Enable</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2315/overview/f02885bb-e043-4a60-8d0c-22242bd77fa9</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2318/overview/39cd0e04-6f9c-40da-b0be-8eaae7f1603d</t>
         </is>
       </c>
       <c r="D206" t="inlineStr">
@@ -12213,7 +12289,7 @@
       </c>
       <c r="M206" t="inlineStr">
         <is>
-          <t>£2.0 million</t>
+          <t>£4.0 million</t>
         </is>
       </c>
       <c r="N206" s="1" t="n">
@@ -12228,21 +12304,21 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Launchpad: life and health sciences, Northern Ireland – Rd3 MFA</t>
+          <t>CAM Pathfinder: Demonstrate</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2305/overview/fe565f48-36a8-4d8b-8515-e89d750f259c</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2315/overview/f02885bb-e043-4a60-8d0c-22242bd77fa9</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>2025-10-16 08:19</t>
+          <t>2025-10-15 08:19</t>
         </is>
       </c>
       <c r="E207" s="1" t="n">
-        <v>45946.34652777778</v>
+        <v>45945.34652777778</v>
       </c>
       <c r="F207" t="b">
         <v>1</v>
@@ -12255,15 +12331,15 @@
       <c r="J207" t="inlineStr"/>
       <c r="K207" t="inlineStr">
         <is>
-          <t>Wednesday 26 November 2025 11:00am</t>
+          <t>Wednesday 17 December 2025 11:00am</t>
         </is>
       </c>
       <c r="L207" s="1" t="n">
-        <v>45987.45833333334</v>
+        <v>46008.45833333334</v>
       </c>
       <c r="M207" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£2.0 million</t>
         </is>
       </c>
       <c r="N207" s="1" t="n">
@@ -12278,21 +12354,21 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>ADOPT Facilitator Support Grant: Round 5</t>
+          <t>Launchpad: life and health sciences, Northern Ireland – Rd3 MFA</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2299/overview/0a26e49f-fa03-4096-aa8b-3eb39b68f20d</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2305/overview/fe565f48-36a8-4d8b-8515-e89d750f259c</t>
         </is>
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>2025-10-17 08:19</t>
+          <t>2025-10-16 08:19</t>
         </is>
       </c>
       <c r="E208" s="1" t="n">
-        <v>45947.34652777778</v>
+        <v>45946.34652777778</v>
       </c>
       <c r="F208" t="b">
         <v>1</v>
@@ -12313,7 +12389,7 @@
       </c>
       <c r="M208" t="inlineStr">
         <is>
-          <t>£2,500</t>
+          <t>£100,000</t>
         </is>
       </c>
       <c r="N208" s="1" t="n">
@@ -12328,21 +12404,21 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Battery Innovation Feasibility Studies Round 1</t>
+          <t>ADOPT Facilitator Support Grant: Round 5</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2313/overview/508ab35f-0e07-4e84-8e31-bbbcb619bc9e</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2299/overview/0a26e49f-fa03-4096-aa8b-3eb39b68f20d</t>
         </is>
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>2025-10-18 08:16</t>
+          <t>2025-10-17 08:19</t>
         </is>
       </c>
       <c r="E209" s="1" t="n">
-        <v>45948.34444444445</v>
+        <v>45947.34652777778</v>
       </c>
       <c r="F209" t="b">
         <v>1</v>
@@ -12355,15 +12431,15 @@
       <c r="J209" t="inlineStr"/>
       <c r="K209" t="inlineStr">
         <is>
-          <t>Wednesday 17 December 2025 11:00am</t>
+          <t>Wednesday 26 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L209" s="1" t="n">
-        <v>46008.45833333334</v>
+        <v>45987.45833333334</v>
       </c>
       <c r="M209" t="inlineStr">
         <is>
-          <t>£500,000</t>
+          <t>£2,500</t>
         </is>
       </c>
       <c r="N209" s="1" t="n">
@@ -12378,12 +12454,12 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Battery Innovation Concept Development Round 1</t>
+          <t>Battery Innovation Feasibility Studies Round 1</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2314/overview/4d1e65d7-b380-41b7-8dcf-b25cd26b9ab5</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2313/overview/508ab35f-0e07-4e84-8e31-bbbcb619bc9e</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
@@ -12413,7 +12489,7 @@
       </c>
       <c r="M210" t="inlineStr">
         <is>
-          <t>£4.0 million</t>
+          <t>£500,000</t>
         </is>
       </c>
       <c r="N210" s="1" t="n">
@@ -12428,21 +12504,21 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>The Agentic AI Pioneers Prize</t>
+          <t>Battery Innovation Concept Development Round 1</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2316/overview/fa0eeab0-3021-4cbc-8975-5bd45a7d642a</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2314/overview/4d1e65d7-b380-41b7-8dcf-b25cd26b9ab5</t>
         </is>
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>2025-10-21 08:20</t>
+          <t>2025-10-18 08:16</t>
         </is>
       </c>
       <c r="E211" s="1" t="n">
-        <v>45951.34722222222</v>
+        <v>45948.34444444445</v>
       </c>
       <c r="F211" t="b">
         <v>1</v>
@@ -12455,13 +12531,17 @@
       <c r="J211" t="inlineStr"/>
       <c r="K211" t="inlineStr">
         <is>
-          <t>Wednesday 19 November 2025 11:00am</t>
+          <t>Wednesday 17 December 2025 11:00am</t>
         </is>
       </c>
       <c r="L211" s="1" t="n">
-        <v>45980.45833333334</v>
-      </c>
-      <c r="M211" t="inlineStr"/>
+        <v>46008.45833333334</v>
+      </c>
+      <c r="M211" t="inlineStr">
+        <is>
+          <t>£4.0 million</t>
+        </is>
+      </c>
       <c r="N211" s="1" t="n">
         <v>45945</v>
       </c>
@@ -12474,21 +12554,21 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>MSI: SME resource and energy efficiency – industrial research</t>
+          <t>The Agentic AI Pioneers Prize</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2328/overview/79cb058a-71b3-459a-93c2-8c96ecf7f18a</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2316/overview/fa0eeab0-3021-4cbc-8975-5bd45a7d642a</t>
         </is>
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>2025-10-22 08:21</t>
+          <t>2025-10-21 08:20</t>
         </is>
       </c>
       <c r="E212" s="1" t="n">
-        <v>45952.34791666667</v>
+        <v>45951.34722222222</v>
       </c>
       <c r="F212" t="b">
         <v>1</v>
@@ -12501,19 +12581,15 @@
       <c r="J212" t="inlineStr"/>
       <c r="K212" t="inlineStr">
         <is>
-          <t>Wednesday 10 December 2025 11:00am</t>
+          <t>Wednesday 19 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L212" s="1" t="n">
-        <v>46001.45833333334</v>
-      </c>
-      <c r="M212" t="inlineStr">
-        <is>
-          <t>£1.0 million</t>
-        </is>
-      </c>
+        <v>45980.45833333334</v>
+      </c>
+      <c r="M212" t="inlineStr"/>
       <c r="N212" s="1" t="n">
-        <v>45952</v>
+        <v>45945</v>
       </c>
     </row>
     <row r="213">
@@ -12524,12 +12600,12 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>MSI: SME resource and energy   efficiency – feasibility studies</t>
+          <t>MSI: SME resource and energy efficiency – industrial research</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2327/overview/bd7d1a37-69dc-4d09-8615-2bae4bcf3666</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2328/overview/79cb058a-71b3-459a-93c2-8c96ecf7f18a</t>
         </is>
       </c>
       <c r="D213" t="inlineStr">
@@ -12559,7 +12635,7 @@
       </c>
       <c r="M213" t="inlineStr">
         <is>
-          <t>£150,000</t>
+          <t>£1.0 million</t>
         </is>
       </c>
       <c r="N213" s="1" t="n">
@@ -12574,21 +12650,21 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Full ADOPT Grant Round 4</t>
+          <t>MSI: SME resource and energy   efficiency – feasibility studies</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2298/overview/71fd7055-502d-4f85-9127-749156a80fe6</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2327/overview/bd7d1a37-69dc-4d09-8615-2bae4bcf3666</t>
         </is>
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>2025-10-23 08:19</t>
+          <t>2025-10-22 08:21</t>
         </is>
       </c>
       <c r="E214" s="1" t="n">
-        <v>45953.34652777778</v>
+        <v>45952.34791666667</v>
       </c>
       <c r="F214" t="b">
         <v>1</v>
@@ -12609,7 +12685,7 @@
       </c>
       <c r="M214" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£150,000</t>
         </is>
       </c>
       <c r="N214" s="1" t="n">
@@ -12624,21 +12700,21 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Innovate UK Innovation Loans Round 24</t>
+          <t>Full ADOPT Grant Round 4</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2322/overview/1b933876-5f58-4dec-85ab-68b8c2722211</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2298/overview/71fd7055-502d-4f85-9127-749156a80fe6</t>
         </is>
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>2025-10-24 08:19</t>
+          <t>2025-10-23 08:19</t>
         </is>
       </c>
       <c r="E215" s="1" t="n">
-        <v>45954.34652777778</v>
+        <v>45953.34652777778</v>
       </c>
       <c r="F215" t="b">
         <v>1</v>
@@ -12651,15 +12727,15 @@
       <c r="J215" t="inlineStr"/>
       <c r="K215" t="inlineStr">
         <is>
-          <t>Wednesday 7 January 2026 11:00am</t>
+          <t>Wednesday 10 December 2025 11:00am</t>
         </is>
       </c>
       <c r="L215" s="1" t="n">
-        <v>46029.45833333334</v>
+        <v>46001.45833333334</v>
       </c>
       <c r="M215" t="inlineStr">
         <is>
-          <t>£5.0 million</t>
+          <t>£100,000</t>
         </is>
       </c>
       <c r="N215" s="1" t="n">
@@ -12674,21 +12750,21 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Knowledge Transfer Partnership (KTP): 2025 – 2026 Round 4</t>
+          <t>Innovate UK Innovation Loans Round 24</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2290/overview/8dd45f5c-3f38-4e38-b733-42b6cf601292</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2322/overview/1b933876-5f58-4dec-85ab-68b8c2722211</t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>2025-10-25 08:16</t>
+          <t>2025-10-24 08:19</t>
         </is>
       </c>
       <c r="E216" s="1" t="n">
-        <v>45955.34444444445</v>
+        <v>45954.34652777778</v>
       </c>
       <c r="F216" t="b">
         <v>1</v>
@@ -12701,15 +12777,15 @@
       <c r="J216" t="inlineStr"/>
       <c r="K216" t="inlineStr">
         <is>
-          <t>Wednesday 26 November 2025 11:00am</t>
+          <t>Wednesday 7 January 2026 11:00am</t>
         </is>
       </c>
       <c r="L216" s="1" t="n">
-        <v>45987.45833333334</v>
+        <v>46029.45833333334</v>
       </c>
       <c r="M216" t="inlineStr">
         <is>
-          <t>£8,500</t>
+          <t>£5.0 million</t>
         </is>
       </c>
       <c r="N216" s="1" t="n">
@@ -12724,21 +12800,21 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>National Materials Innovation Programme: Feasibility Studies</t>
+          <t>Knowledge Transfer Partnership (KTP): 2025 – 2026 Round 4</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2326/overview/ca8aab61-a03b-431f-94a8-5c9b008495d5</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2290/overview/8dd45f5c-3f38-4e38-b733-42b6cf601292</t>
         </is>
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>2025-10-31 08:18</t>
+          <t>2025-10-25 08:16</t>
         </is>
       </c>
       <c r="E217" s="1" t="n">
-        <v>45961.34583333333</v>
+        <v>45955.34444444445</v>
       </c>
       <c r="F217" t="b">
         <v>1</v>
@@ -12751,19 +12827,19 @@
       <c r="J217" t="inlineStr"/>
       <c r="K217" t="inlineStr">
         <is>
-          <t>Wednesday 17 December 2025 11:00am</t>
+          <t>Wednesday 26 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L217" s="1" t="n">
-        <v>46008.45833333334</v>
+        <v>45987.45833333334</v>
       </c>
       <c r="M217" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£8,500</t>
         </is>
       </c>
       <c r="N217" s="1" t="n">
-        <v>45959</v>
+        <v>45952</v>
       </c>
     </row>
     <row r="218">
@@ -12774,21 +12850,21 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>UK-Canada Quantum Communications and Networking Demonstrator</t>
+          <t>National Materials Innovation Programme: Feasibility Studies</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2335/overview/64e26f1b-8564-4539-b3ca-1b15ebf4f94a</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2326/overview/ca8aab61-a03b-431f-94a8-5c9b008495d5</t>
         </is>
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>2025-11-04 08:20</t>
+          <t>2025-10-31 08:18</t>
         </is>
       </c>
       <c r="E218" s="1" t="n">
-        <v>45965.34722222222</v>
+        <v>45961.34583333333</v>
       </c>
       <c r="F218" t="b">
         <v>1</v>
@@ -12801,15 +12877,15 @@
       <c r="J218" t="inlineStr"/>
       <c r="K218" t="inlineStr">
         <is>
-          <t>Wednesday 26 November 2025 11:00am</t>
+          <t>Wednesday 17 December 2025 11:00am</t>
         </is>
       </c>
       <c r="L218" s="1" t="n">
-        <v>45987.45833333334</v>
+        <v>46008.45833333334</v>
       </c>
       <c r="M218" t="inlineStr">
         <is>
-          <t>£3.4 million</t>
+          <t>£100,000</t>
         </is>
       </c>
       <c r="N218" s="1" t="n">
@@ -12824,12 +12900,12 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Increasing EV charging capacity on the strategic road network</t>
+          <t>UK-Canada Quantum Communications and Networking Demonstrator</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2304/overview/9ea6670e-83fd-43f9-972f-e0eff8fe77a8</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2335/overview/64e26f1b-8564-4539-b3ca-1b15ebf4f94a</t>
         </is>
       </c>
       <c r="D219" t="inlineStr">
@@ -12851,15 +12927,15 @@
       <c r="J219" t="inlineStr"/>
       <c r="K219" t="inlineStr">
         <is>
-          <t>Wednesday 25 March 2026 11:00am</t>
+          <t>Wednesday 26 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L219" s="1" t="n">
-        <v>46106.45833333334</v>
+        <v>45987.45833333334</v>
       </c>
       <c r="M219" t="inlineStr">
         <is>
-          <t>£3.0 million</t>
+          <t>£3.4 million</t>
         </is>
       </c>
       <c r="N219" s="1" t="n">
@@ -12874,21 +12950,21 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Biomedical Catalyst 2025: Industry led R&amp;D small projects</t>
+          <t>Increasing EV charging capacity on the strategic road network</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2333/overview/f5431c75-e2e1-48f4-bc8e-62d52121cb6f</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2304/overview/9ea6670e-83fd-43f9-972f-e0eff8fe77a8</t>
         </is>
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>2025-11-05 08:19</t>
+          <t>2025-11-04 08:20</t>
         </is>
       </c>
       <c r="E220" s="1" t="n">
-        <v>45966.34652777778</v>
+        <v>45965.34722222222</v>
       </c>
       <c r="F220" t="b">
         <v>1</v>
@@ -12901,19 +12977,19 @@
       <c r="J220" t="inlineStr"/>
       <c r="K220" t="inlineStr">
         <is>
-          <t>Wednesday 10 December 2025 11:00am</t>
+          <t>Wednesday 25 March 2026 11:00am</t>
         </is>
       </c>
       <c r="L220" s="1" t="n">
-        <v>46001.45833333334</v>
+        <v>46106.45833333334</v>
       </c>
       <c r="M220" t="inlineStr">
         <is>
-          <t>£1.0 million</t>
+          <t>£3.0 million</t>
         </is>
       </c>
       <c r="N220" s="1" t="n">
-        <v>45966</v>
+        <v>45959</v>
       </c>
     </row>
     <row r="221">
@@ -12924,12 +13000,12 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Biomedical Catalyst 2025: Industry led R&amp;D large projects</t>
+          <t>Biomedical Catalyst 2025: Industry led R&amp;D small projects</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2332/overview/bf6bd8c3-e550-478d-b374-a3cb0fb4d3d3</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2333/overview/f5431c75-e2e1-48f4-bc8e-62d52121cb6f</t>
         </is>
       </c>
       <c r="D221" t="inlineStr">
@@ -12959,7 +13035,7 @@
       </c>
       <c r="M221" t="inlineStr">
         <is>
-          <t>£4.0 million</t>
+          <t>£1.0 million</t>
         </is>
       </c>
       <c r="N221" s="1" t="n">
@@ -12974,12 +13050,12 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>ATI Programme strategic batch EoI – November 2025</t>
+          <t>Biomedical Catalyst 2025: Industry led R&amp;D large projects</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2334/overview/4af06b80-2953-4cb3-8cc0-987ec5a2f322</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2332/overview/bf6bd8c3-e550-478d-b374-a3cb0fb4d3d3</t>
         </is>
       </c>
       <c r="D222" t="inlineStr">
@@ -13001,13 +13077,17 @@
       <c r="J222" t="inlineStr"/>
       <c r="K222" t="inlineStr">
         <is>
-          <t>Wednesday 19 November 2025 11:00am</t>
+          <t>Wednesday 10 December 2025 11:00am</t>
         </is>
       </c>
       <c r="L222" s="1" t="n">
-        <v>45980.45833333334</v>
-      </c>
-      <c r="M222" t="inlineStr"/>
+        <v>46001.45833333334</v>
+      </c>
+      <c r="M222" t="inlineStr">
+        <is>
+          <t>£4.0 million</t>
+        </is>
+      </c>
       <c r="N222" s="1" t="n">
         <v>45966</v>
       </c>
@@ -13020,21 +13100,21 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>DRIVE35 Scale-up: Feasibility Studies 2</t>
+          <t>ATI Programme strategic batch EoI – November 2025</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2341/overview/4b0efce9-75b8-4e84-97c0-fc6277396586</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2334/overview/4af06b80-2953-4cb3-8cc0-987ec5a2f322</t>
         </is>
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>2025-11-11 08:19</t>
+          <t>2025-11-05 08:19</t>
         </is>
       </c>
       <c r="E223" s="1" t="n">
-        <v>45972.34652777778</v>
+        <v>45966.34652777778</v>
       </c>
       <c r="F223" t="b">
         <v>1</v>
@@ -13047,17 +13127,13 @@
       <c r="J223" t="inlineStr"/>
       <c r="K223" t="inlineStr">
         <is>
-          <t>Wednesday 17 December 2025 11:00am</t>
+          <t>Wednesday 19 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L223" s="1" t="n">
-        <v>46008.45833333334</v>
-      </c>
-      <c r="M223" t="inlineStr">
-        <is>
-          <t>£750,000</t>
-        </is>
-      </c>
+        <v>45980.45833333334</v>
+      </c>
+      <c r="M223" t="inlineStr"/>
       <c r="N223" s="1" t="n">
         <v>45966</v>
       </c>
@@ -13070,21 +13146,21 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Women in Innovation Awards 2025/26</t>
+          <t>DRIVE35 Scale-up: Feasibility Studies 2</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2337/overview/3750b1cd-2080-4a1c-82c0-003fbaafdd2d</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2341/overview/4b0efce9-75b8-4e84-97c0-fc6277396586</t>
         </is>
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>2025-11-27 13:23</t>
+          <t>2025-11-11 08:19</t>
         </is>
       </c>
       <c r="E224" s="1" t="n">
-        <v>45988.55763888889</v>
+        <v>45972.34652777778</v>
       </c>
       <c r="F224" t="b">
         <v>1</v>
@@ -13097,19 +13173,19 @@
       <c r="J224" t="inlineStr"/>
       <c r="K224" t="inlineStr">
         <is>
-          <t>Wednesday 4 February 2026 11:00am</t>
+          <t>Wednesday 17 December 2025 11:00am</t>
         </is>
       </c>
       <c r="L224" s="1" t="n">
-        <v>46057.45833333334</v>
+        <v>46008.45833333334</v>
       </c>
       <c r="M224" t="inlineStr">
         <is>
-          <t>£75,000</t>
+          <t>£750,000</t>
         </is>
       </c>
       <c r="N224" s="1" t="n">
-        <v>45987</v>
+        <v>45966</v>
       </c>
     </row>
     <row r="225">
@@ -13120,21 +13196,21 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Knowledge Transfer Partnership (KTP): 2025 – 2026 Round 5</t>
+          <t>Women in Innovation Awards 2025/26</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2354/overview/c7008321-f651-45c5-a409-c3215231fbb4</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2337/overview/3750b1cd-2080-4a1c-82c0-003fbaafdd2d</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>2025-12-02 08:22</t>
+          <t>2025-11-27 13:23</t>
         </is>
       </c>
       <c r="E225" s="1" t="n">
-        <v>45993.34861111111</v>
+        <v>45988.55763888889</v>
       </c>
       <c r="F225" t="b">
         <v>1</v>
@@ -13155,7 +13231,7 @@
       </c>
       <c r="M225" t="inlineStr">
         <is>
-          <t>£8,500</t>
+          <t>£75,000</t>
         </is>
       </c>
       <c r="N225" s="1" t="n">
@@ -13170,21 +13246,21 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Innovate UK Growth Catalyst – Investor Partnerships Round 2</t>
+          <t>Knowledge Transfer Partnership (KTP): 2025 – 2026 Round 5</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2360/overview/37d8f6e1-5600-4e9e-bbfc-11bc320f8808</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2354/overview/c7008321-f651-45c5-a409-c3215231fbb4</t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>2025-12-11 08:22</t>
+          <t>2025-12-02 08:22</t>
         </is>
       </c>
       <c r="E226" s="1" t="n">
-        <v>46002.34861111111</v>
+        <v>45993.34861111111</v>
       </c>
       <c r="F226" t="b">
         <v>1</v>
@@ -13197,19 +13273,19 @@
       <c r="J226" t="inlineStr"/>
       <c r="K226" t="inlineStr">
         <is>
-          <t>Tuesday 3 February 2026 11:00am</t>
+          <t>Wednesday 4 February 2026 11:00am</t>
         </is>
       </c>
       <c r="L226" s="1" t="n">
-        <v>46056.45833333334</v>
+        <v>46057.45833333334</v>
       </c>
       <c r="M226" t="inlineStr">
         <is>
-          <t>£2.0 million</t>
+          <t>£8,500</t>
         </is>
       </c>
       <c r="N226" s="1" t="n">
-        <v>46001</v>
+        <v>45987</v>
       </c>
     </row>
     <row r="227">
@@ -13220,21 +13296,21 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Full ADOPT Grant: Round 5</t>
+          <t>Innovate UK Growth Catalyst – Investor Partnerships Round 2</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2358/overview/f93f32c2-dd04-474d-bc35-a8af1ecac1a9</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2360/overview/37d8f6e1-5600-4e9e-bbfc-11bc320f8808</t>
         </is>
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>2025-12-12 08:22</t>
+          <t>2025-12-11 08:22</t>
         </is>
       </c>
       <c r="E227" s="1" t="n">
-        <v>46003.34861111111</v>
+        <v>46002.34861111111</v>
       </c>
       <c r="F227" t="b">
         <v>1</v>
@@ -13247,15 +13323,15 @@
       <c r="J227" t="inlineStr"/>
       <c r="K227" t="inlineStr">
         <is>
-          <t>Wednesday 4 February 2026 11:00am</t>
+          <t>Tuesday 3 February 2026 11:00am</t>
         </is>
       </c>
       <c r="L227" s="1" t="n">
-        <v>46057.45833333334</v>
+        <v>46056.45833333334</v>
       </c>
       <c r="M227" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£2.0 million</t>
         </is>
       </c>
       <c r="N227" s="1" t="n">
@@ -13270,21 +13346,21 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>ADOPT Facilitator Support Grant: Round 6</t>
+          <t>Full ADOPT Grant: Round 5</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2371/overview/471bfe91-9f9c-4086-a28a-15296f1957e2</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2358/overview/f93f32c2-dd04-474d-bc35-a8af1ecac1a9</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>2025-12-18 08:21</t>
+          <t>2025-12-12 08:22</t>
         </is>
       </c>
       <c r="E228" s="1" t="n">
-        <v>46009.34791666667</v>
+        <v>46003.34861111111</v>
       </c>
       <c r="F228" t="b">
         <v>1</v>
@@ -13297,19 +13373,19 @@
       <c r="J228" t="inlineStr"/>
       <c r="K228" t="inlineStr">
         <is>
-          <t>Wednesday 25 February 2026 11:00am</t>
+          <t>Wednesday 4 February 2026 11:00am</t>
         </is>
       </c>
       <c r="L228" s="1" t="n">
-        <v>46078.45833333334</v>
+        <v>46057.45833333334</v>
       </c>
       <c r="M228" t="inlineStr">
         <is>
-          <t>£2,500</t>
+          <t>£100,000</t>
         </is>
       </c>
       <c r="N228" s="1" t="n">
-        <v>46008</v>
+        <v>46001</v>
       </c>
     </row>
     <row r="229">
@@ -13320,12 +13396,12 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Commercialising Knowledge Assets Fund (CKAF) Spring</t>
+          <t>ADOPT Facilitator Support Grant: Round 6</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2369/overview/abf7d399-81b9-4f33-b592-51825a288c37</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2371/overview/471bfe91-9f9c-4086-a28a-15296f1957e2</t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
@@ -13347,15 +13423,15 @@
       <c r="J229" t="inlineStr"/>
       <c r="K229" t="inlineStr">
         <is>
-          <t>Thursday 7 May 2026 11:00am</t>
+          <t>Wednesday 25 February 2026 11:00am</t>
         </is>
       </c>
       <c r="L229" s="1" t="n">
-        <v>46149.45833333334</v>
+        <v>46078.45833333334</v>
       </c>
       <c r="M229" t="inlineStr">
         <is>
-          <t>£250,000</t>
+          <t>£2,500</t>
         </is>
       </c>
       <c r="N229" s="1" t="n">
@@ -13370,21 +13446,21 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Energy catalyst round 11 – mid stage</t>
+          <t>Commercialising Knowledge Assets Fund (CKAF) Spring</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2363/overview/9f759af1-3732-4d15-995d-053e28025d22</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2369/overview/abf7d399-81b9-4f33-b592-51825a288c37</t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>2026-01-06 08:22</t>
+          <t>2025-12-18 08:21</t>
         </is>
       </c>
       <c r="E230" s="1" t="n">
-        <v>46028.34861111111</v>
+        <v>46009.34791666667</v>
       </c>
       <c r="F230" t="b">
         <v>1</v>
@@ -13397,19 +13473,19 @@
       <c r="J230" t="inlineStr"/>
       <c r="K230" t="inlineStr">
         <is>
-          <t>Wednesday 25 March 2026 11:00am</t>
+          <t>Thursday 7 May 2026 11:00am</t>
         </is>
       </c>
       <c r="L230" s="1" t="n">
-        <v>46106.45833333334</v>
+        <v>46149.45833333334</v>
       </c>
       <c r="M230" t="inlineStr">
         <is>
-          <t>£1.5 million</t>
+          <t>£250,000</t>
         </is>
       </c>
       <c r="N230" s="1" t="n">
-        <v>46022</v>
+        <v>46008</v>
       </c>
     </row>
     <row r="231">
@@ -13420,12 +13496,12 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Energy catalyst round 11 – late stage</t>
+          <t>Energy catalyst round 11 – mid stage</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2364/overview/b9d4dedf-d22a-41d1-9ca2-6c5a279519be</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2363/overview/9f759af1-3732-4d15-995d-053e28025d22</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
@@ -13455,7 +13531,7 @@
       </c>
       <c r="M231" t="inlineStr">
         <is>
-          <t>£5.0 million</t>
+          <t>£1.5 million</t>
         </is>
       </c>
       <c r="N231" s="1" t="n">
@@ -13470,12 +13546,12 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Energy catalyst round 11 – early stage</t>
+          <t>Energy catalyst round 11 – late stage</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2362/overview/640b2f4e-8571-4aef-9e2a-67e35db3db77</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2364/overview/b9d4dedf-d22a-41d1-9ca2-6c5a279519be</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
@@ -13505,7 +13581,7 @@
       </c>
       <c r="M232" t="inlineStr">
         <is>
-          <t>£300,000</t>
+          <t>£5.0 million</t>
         </is>
       </c>
       <c r="N232" s="1" t="n">
@@ -13520,12 +13596,12 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>DRIVE35 Innovation Fund: Demonstrate 2</t>
+          <t>Energy catalyst round 11 – early stage</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2351/overview/349c38f5-5ed2-4cf4-a324-bda2d6cd1e67</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2362/overview/640b2f4e-8571-4aef-9e2a-67e35db3db77</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
@@ -13547,15 +13623,15 @@
       <c r="J233" t="inlineStr"/>
       <c r="K233" t="inlineStr">
         <is>
-          <t>Wednesday 11 March 2026 11:00am</t>
+          <t>Wednesday 25 March 2026 11:00am</t>
         </is>
       </c>
       <c r="L233" s="1" t="n">
-        <v>46092.45833333334</v>
+        <v>46106.45833333334</v>
       </c>
       <c r="M233" t="inlineStr">
         <is>
-          <t>£1.5 million</t>
+          <t>£300,000</t>
         </is>
       </c>
       <c r="N233" s="1" t="n">
@@ -13570,12 +13646,12 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>DRIVE35 Innovation Fund: Collaborate 2</t>
+          <t>DRIVE35 Innovation Fund: Demonstrate 2</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2350/overview/dbd41be3-14ea-4c83-8774-eb28a8703d57</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2351/overview/349c38f5-5ed2-4cf4-a324-bda2d6cd1e67</t>
         </is>
       </c>
       <c r="D234" t="inlineStr">
@@ -13597,15 +13673,15 @@
       <c r="J234" t="inlineStr"/>
       <c r="K234" t="inlineStr">
         <is>
-          <t>Wednesday 18 March 2026 11:00am</t>
+          <t>Wednesday 11 March 2026 11:00am</t>
         </is>
       </c>
       <c r="L234" s="1" t="n">
-        <v>46099.45833333334</v>
+        <v>46092.45833333334</v>
       </c>
       <c r="M234" t="inlineStr">
         <is>
-          <t>£25.0 million</t>
+          <t>£1.5 million</t>
         </is>
       </c>
       <c r="N234" s="1" t="n">
@@ -13620,21 +13696,21 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Innovate UK Innovation Loans Round 25</t>
+          <t>DRIVE35 Innovation Fund: Collaborate 2</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2373/overview/609dc5dd-d3e8-4f51-af3a-3eb1b3314710</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2350/overview/dbd41be3-14ea-4c83-8774-eb28a8703d57</t>
         </is>
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>2026-01-08 08:22</t>
+          <t>2026-01-06 08:22</t>
         </is>
       </c>
       <c r="E235" s="1" t="n">
-        <v>46030.34861111111</v>
+        <v>46028.34861111111</v>
       </c>
       <c r="F235" t="b">
         <v>1</v>
@@ -13647,19 +13723,19 @@
       <c r="J235" t="inlineStr"/>
       <c r="K235" t="inlineStr">
         <is>
-          <t>Wednesday 4 March 2026 11:00am</t>
+          <t>Wednesday 18 March 2026 11:00am</t>
         </is>
       </c>
       <c r="L235" s="1" t="n">
-        <v>46085.45833333334</v>
+        <v>46099.45833333334</v>
       </c>
       <c r="M235" t="inlineStr">
         <is>
-          <t>£5.0 million</t>
+          <t>£25.0 million</t>
         </is>
       </c>
       <c r="N235" s="1" t="n">
-        <v>46029</v>
+        <v>46022</v>
       </c>
     </row>
     <row r="236">
@@ -13670,21 +13746,21 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Cyber Security Academic Startup Accelerator Programme Y10 Phase 1</t>
+          <t>Innovate UK Innovation Loans Round 25</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2376/overview/1b9b9265-ca4b-4f8c-a0c2-577cb8713642</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2373/overview/609dc5dd-d3e8-4f51-af3a-3eb1b3314710</t>
         </is>
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>2026-01-15 08:23</t>
+          <t>2026-01-08 08:22</t>
         </is>
       </c>
       <c r="E236" s="1" t="n">
-        <v>46037.34930555556</v>
+        <v>46030.34861111111</v>
       </c>
       <c r="F236" t="b">
         <v>1</v>
@@ -13697,19 +13773,19 @@
       <c r="J236" t="inlineStr"/>
       <c r="K236" t="inlineStr">
         <is>
-          <t>Wednesday 11 February 2026 11:00am</t>
+          <t>Wednesday 4 March 2026 11:00am</t>
         </is>
       </c>
       <c r="L236" s="1" t="n">
-        <v>46064.45833333334</v>
+        <v>46085.45833333334</v>
       </c>
       <c r="M236" t="inlineStr">
         <is>
-          <t>£32,000</t>
+          <t>£5.0 million</t>
         </is>
       </c>
       <c r="N236" s="1" t="n">
-        <v>46036</v>
+        <v>46029</v>
       </c>
     </row>
     <row r="237">
@@ -13720,21 +13796,21 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Ofgem Strategic Innovation Fund Round 5 Discovery C5</t>
+          <t>Cyber Security Academic Startup Accelerator Programme Y10 Phase 1</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2346/overview/e172ee7c-3050-4d47-bf11-235cfe76c1e1</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2376/overview/1b9b9265-ca4b-4f8c-a0c2-577cb8713642</t>
         </is>
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>2026-01-20 08:24</t>
+          <t>2026-01-15 08:23</t>
         </is>
       </c>
       <c r="E237" s="1" t="n">
-        <v>46042.35</v>
+        <v>46037.34930555556</v>
       </c>
       <c r="F237" t="b">
         <v>1</v>
@@ -13747,15 +13823,15 @@
       <c r="J237" t="inlineStr"/>
       <c r="K237" t="inlineStr">
         <is>
-          <t>Wednesday 25 February 2026 11:00am</t>
+          <t>Wednesday 11 February 2026 11:00am</t>
         </is>
       </c>
       <c r="L237" s="1" t="n">
-        <v>46078.45833333334</v>
+        <v>46064.45833333334</v>
       </c>
       <c r="M237" t="inlineStr">
         <is>
-          <t>£150,000</t>
+          <t>£32,000</t>
         </is>
       </c>
       <c r="N237" s="1" t="n">
@@ -13770,21 +13846,21 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Advanced manufacturing supply chain innovation FS</t>
+          <t>Ofgem Strategic Innovation Fund Round 5 Discovery C5</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2384/overview/2ad8ce21-d3f6-48bf-b55a-5af2a892a1e0</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2346/overview/e172ee7c-3050-4d47-bf11-235cfe76c1e1</t>
         </is>
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>2026-01-26 12:10</t>
+          <t>2026-01-20 08:24</t>
         </is>
       </c>
       <c r="E238" s="1" t="n">
-        <v>46048.50694444445</v>
+        <v>46042.35</v>
       </c>
       <c r="F238" t="b">
         <v>1</v>
@@ -13797,19 +13873,19 @@
       <c r="J238" t="inlineStr"/>
       <c r="K238" t="inlineStr">
         <is>
-          <t>Wednesday 11 March 2026 11:00am</t>
+          <t>Wednesday 25 February 2026 11:00am</t>
         </is>
       </c>
       <c r="L238" s="1" t="n">
-        <v>46092.45833333334</v>
+        <v>46078.45833333334</v>
       </c>
       <c r="M238" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£150,000</t>
         </is>
       </c>
       <c r="N238" s="1" t="n">
-        <v>46043</v>
+        <v>46036</v>
       </c>
     </row>
     <row r="239">
@@ -13820,21 +13896,21 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>TechLocal: Connecting Local Talent to Local Tech Jobs</t>
+          <t>Advanced manufacturing supply chain innovation FS</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2378/overview/ae120ce2-7b72-4cf2-8dde-f78b02d5996d</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2384/overview/2ad8ce21-d3f6-48bf-b55a-5af2a892a1e0</t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>2026-01-28 10:24</t>
+          <t>2026-01-26 12:10</t>
         </is>
       </c>
       <c r="E239" s="1" t="n">
-        <v>46050.43333333333</v>
+        <v>46048.50694444445</v>
       </c>
       <c r="F239" t="b">
         <v>1</v>
@@ -13847,19 +13923,19 @@
       <c r="J239" t="inlineStr"/>
       <c r="K239" t="inlineStr">
         <is>
-          <t>Wednesday 18 March 2026 11:00am</t>
+          <t>Wednesday 11 March 2026 11:00am</t>
         </is>
       </c>
       <c r="L239" s="1" t="n">
-        <v>46099.45833333334</v>
+        <v>46092.45833333334</v>
       </c>
       <c r="M239" t="inlineStr">
         <is>
-          <t>£225,000</t>
+          <t>£100,000</t>
         </is>
       </c>
       <c r="N239" s="1" t="n">
-        <v>46050</v>
+        <v>46043</v>
       </c>
     </row>
     <row r="240">
@@ -13870,12 +13946,12 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>TechLocal AI Professional Degree and Traineeship Accelerator</t>
+          <t>TechLocal: Connecting Local Talent to Local Tech Jobs</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2375/overview/6431359e-eb5c-4f76-b49d-299948107fbd</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2378/overview/ae120ce2-7b72-4cf2-8dde-f78b02d5996d</t>
         </is>
       </c>
       <c r="D240" t="inlineStr">
@@ -13905,7 +13981,7 @@
       </c>
       <c r="M240" t="inlineStr">
         <is>
-          <t>£300,000</t>
+          <t>£225,000</t>
         </is>
       </c>
       <c r="N240" s="1" t="n">
@@ -13920,21 +13996,21 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Robotics Adoption Programme skills development</t>
+          <t>TechLocal AI Professional Degree and Traineeship Accelerator</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2387/overview/daca31c2-8395-4bc2-a5da-55eb1e432fa4</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2375/overview/6431359e-eb5c-4f76-b49d-299948107fbd</t>
         </is>
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>2026-02-02 10:39</t>
+          <t>2026-01-28 10:24</t>
         </is>
       </c>
       <c r="E241" s="1" t="n">
-        <v>46055.44375</v>
+        <v>46050.43333333333</v>
       </c>
       <c r="F241" t="b">
         <v>1</v>
@@ -13947,15 +14023,15 @@
       <c r="J241" t="inlineStr"/>
       <c r="K241" t="inlineStr">
         <is>
-          <t>Wednesday 25 March 2026 11:00am</t>
+          <t>Wednesday 18 March 2026 11:00am</t>
         </is>
       </c>
       <c r="L241" s="1" t="n">
-        <v>46106.45833333334</v>
+        <v>46099.45833333334</v>
       </c>
       <c r="M241" t="inlineStr">
         <is>
-          <t>£500,000</t>
+          <t>£300,000</t>
         </is>
       </c>
       <c r="N241" s="1" t="n">
@@ -13970,21 +14046,21 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Knowledge Transfer Partnership (KTP): 2026 – 2027 Round 1</t>
+          <t>Robotics Adoption Programme skills development</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2380/overview/3e170dd3-4458-4c7e-a096-e0ea50b88040</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2387/overview/daca31c2-8395-4bc2-a5da-55eb1e432fa4</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>2026-02-03 10:35</t>
+          <t>2026-02-02 10:39</t>
         </is>
       </c>
       <c r="E242" s="1" t="n">
-        <v>46056.44097222222</v>
+        <v>46055.44375</v>
       </c>
       <c r="F242" t="b">
         <v>1</v>
@@ -13997,15 +14073,15 @@
       <c r="J242" t="inlineStr"/>
       <c r="K242" t="inlineStr">
         <is>
-          <t>Wednesday 1 April 2026 11:00am</t>
+          <t>Wednesday 25 March 2026 11:00am</t>
         </is>
       </c>
       <c r="L242" s="1" t="n">
-        <v>46113.45833333334</v>
+        <v>46106.45833333334</v>
       </c>
       <c r="M242" t="inlineStr">
         <is>
-          <t>£8,500</t>
+          <t>£500,000</t>
         </is>
       </c>
       <c r="N242" s="1" t="n">
@@ -14020,12 +14096,12 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Biomedical Catalyst Accelerator Provider Pool EoI: late stage</t>
+          <t>Knowledge Transfer Partnership (KTP): 2026 – 2027 Round 1</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2389/overview/a7f7d874-8b6b-45d6-b1e1-1e88e11a1ea5</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2380/overview/3e170dd3-4458-4c7e-a096-e0ea50b88040</t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
@@ -14047,13 +14123,17 @@
       <c r="J243" t="inlineStr"/>
       <c r="K243" t="inlineStr">
         <is>
-          <t>Wednesday 4 March 2026 11:00am</t>
+          <t>Wednesday 1 April 2026 11:00am</t>
         </is>
       </c>
       <c r="L243" s="1" t="n">
-        <v>46085.45833333334</v>
-      </c>
-      <c r="M243" t="inlineStr"/>
+        <v>46113.45833333334</v>
+      </c>
+      <c r="M243" t="inlineStr">
+        <is>
+          <t>£8,500</t>
+        </is>
+      </c>
       <c r="N243" s="1" t="n">
         <v>46050</v>
       </c>
@@ -14066,12 +14146,12 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Biomedical Catalyst Accelerator Provider Pool EoI: early stage</t>
+          <t>Biomedical Catalyst Accelerator Provider Pool EoI: late stage</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2388/overview/08b8ab63-085d-4d79-ae83-e8c1698cb327</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2389/overview/a7f7d874-8b6b-45d6-b1e1-1e88e11a1ea5</t>
         </is>
       </c>
       <c r="D244" t="inlineStr">
@@ -14112,21 +14192,21 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Full ADOPT Grant: Round 6</t>
+          <t>Biomedical Catalyst Accelerator Provider Pool EoI: early stage</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2385/overview/2343c344-807d-41a1-9551-05ac5420ba11</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2388/overview/08b8ab63-085d-4d79-ae83-e8c1698cb327</t>
         </is>
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>2026-02-09 10:53</t>
+          <t>2026-02-03 10:35</t>
         </is>
       </c>
       <c r="E245" s="1" t="n">
-        <v>46062.45347222222</v>
+        <v>46056.44097222222</v>
       </c>
       <c r="F245" t="b">
         <v>1</v>
@@ -14139,19 +14219,15 @@
       <c r="J245" t="inlineStr"/>
       <c r="K245" t="inlineStr">
         <is>
-          <t>Wednesday 8 April 2026 11:00am</t>
+          <t>Wednesday 4 March 2026 11:00am</t>
         </is>
       </c>
       <c r="L245" s="1" t="n">
-        <v>46120.45833333334</v>
-      </c>
-      <c r="M245" t="inlineStr">
-        <is>
-          <t>£100,000</t>
-        </is>
-      </c>
+        <v>46085.45833333334</v>
+      </c>
+      <c r="M245" t="inlineStr"/>
       <c r="N245" s="1" t="n">
-        <v>46057</v>
+        <v>46050</v>
       </c>
     </row>
     <row r="246">
@@ -14162,21 +14238,21 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Zero Emission Flight Demonstrator Round 1</t>
+          <t>Full ADOPT Grant: Round 6</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2397/overview/752074ec-5f01-46d8-863f-596300a11651</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2385/overview/2343c344-807d-41a1-9551-05ac5420ba11</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>2026-02-12 10:40</t>
+          <t>2026-02-09 10:53</t>
         </is>
       </c>
       <c r="E246" s="1" t="n">
-        <v>46065.44444444445</v>
+        <v>46062.45347222222</v>
       </c>
       <c r="F246" t="b">
         <v>1</v>
@@ -14189,19 +14265,19 @@
       <c r="J246" t="inlineStr"/>
       <c r="K246" t="inlineStr">
         <is>
-          <t>Wednesday 1 April 2026 11:00am</t>
+          <t>Wednesday 8 April 2026 11:00am</t>
         </is>
       </c>
       <c r="L246" s="1" t="n">
-        <v>46113.45833333334</v>
+        <v>46120.45833333334</v>
       </c>
       <c r="M246" t="inlineStr">
         <is>
-          <t>£5.0 million</t>
+          <t>£100,000</t>
         </is>
       </c>
       <c r="N246" s="1" t="n">
-        <v>46064</v>
+        <v>46057</v>
       </c>
     </row>
     <row r="247">
@@ -14212,12 +14288,12 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Contracts for Innovation in drug and alcohol addiction healthcare</t>
+          <t>Zero Emission Flight Demonstrator Round 1</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2395/overview/3d49fbc4-6e09-4dd8-9ac8-8e5f88facd8d</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2397/overview/752074ec-5f01-46d8-863f-596300a11651</t>
         </is>
       </c>
       <c r="D247" t="inlineStr">
@@ -14239,15 +14315,15 @@
       <c r="J247" t="inlineStr"/>
       <c r="K247" t="inlineStr">
         <is>
-          <t>Wednesday 6 May 2026 11:00am</t>
+          <t>Wednesday 1 April 2026 11:00am</t>
         </is>
       </c>
       <c r="L247" s="1" t="n">
-        <v>46148.45833333334</v>
+        <v>46113.45833333334</v>
       </c>
       <c r="M247" t="inlineStr">
         <is>
-          <t>£1.5 million</t>
+          <t>£5.0 million</t>
         </is>
       </c>
       <c r="N247" s="1" t="n">
@@ -14262,12 +14338,12 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Advancing innovation in drug and alcohol addiction healthcare</t>
+          <t>Contracts for Innovation in drug and alcohol addiction healthcare</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2394/overview/33b56af8-353f-46ac-bb66-a0928731c0fc</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2395/overview/3d49fbc4-6e09-4dd8-9ac8-8e5f88facd8d</t>
         </is>
       </c>
       <c r="D248" t="inlineStr">
@@ -14297,7 +14373,7 @@
       </c>
       <c r="M248" t="inlineStr">
         <is>
-          <t>£10.0 million</t>
+          <t>£1.5 million</t>
         </is>
       </c>
       <c r="N248" s="1" t="n">
@@ -14312,21 +14388,21 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>UK-Germany Collaborative Innovation for Quantum Technologies 2026</t>
+          <t>Advancing innovation in drug and alcohol addiction healthcare</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2392/overview/b8b93732-6326-4aed-9af3-334e4cc5ecc0</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2394/overview/33b56af8-353f-46ac-bb66-a0928731c0fc</t>
         </is>
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>2026-02-13 10:35</t>
+          <t>2026-02-12 10:40</t>
         </is>
       </c>
       <c r="E249" s="1" t="n">
-        <v>46066.44097222222</v>
+        <v>46065.44444444445</v>
       </c>
       <c r="F249" t="b">
         <v>1</v>
@@ -14339,15 +14415,15 @@
       <c r="J249" t="inlineStr"/>
       <c r="K249" t="inlineStr">
         <is>
-          <t>Wednesday 15 April 2026 11:00am</t>
+          <t>Wednesday 6 May 2026 11:00am</t>
         </is>
       </c>
       <c r="L249" s="1" t="n">
-        <v>46127.45833333334</v>
+        <v>46148.45833333334</v>
       </c>
       <c r="M249" t="inlineStr">
         <is>
-          <t>£1.0 million</t>
+          <t>£10.0 million</t>
         </is>
       </c>
       <c r="N249" s="1" t="n">
@@ -14362,21 +14438,21 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: industrial human relevant drug models</t>
+          <t>UK-Germany Collaborative Innovation for Quantum Technologies 2026</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2396/overview/d55398bb-ff62-43b9-9ee1-bf3fa4b95c5c</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2392/overview/b8b93732-6326-4aed-9af3-334e4cc5ecc0</t>
         </is>
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>2026-02-17 10:40</t>
+          <t>2026-02-13 10:35</t>
         </is>
       </c>
       <c r="E250" s="1" t="n">
-        <v>46070.44444444445</v>
+        <v>46066.44097222222</v>
       </c>
       <c r="F250" t="b">
         <v>1</v>
@@ -14397,10 +14473,60 @@
       </c>
       <c r="M250" t="inlineStr">
         <is>
+          <t>£1.0 million</t>
+        </is>
+      </c>
+      <c r="N250" s="1" t="n">
+        <v>46064</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>Innovate Funding Service</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Contracts for Innovation: industrial human relevant drug models</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2396/overview/d55398bb-ff62-43b9-9ee1-bf3fa4b95c5c</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>2026-02-17 10:40</t>
+        </is>
+      </c>
+      <c r="E251" s="1" t="n">
+        <v>46070.44444444445</v>
+      </c>
+      <c r="F251" t="b">
+        <v>1</v>
+      </c>
+      <c r="G251" t="inlineStr"/>
+      <c r="H251" t="b">
+        <v>0</v>
+      </c>
+      <c r="I251" t="inlineStr"/>
+      <c r="J251" t="inlineStr"/>
+      <c r="K251" t="inlineStr">
+        <is>
+          <t>Wednesday 15 April 2026 11:00am</t>
+        </is>
+      </c>
+      <c r="L251" s="1" t="n">
+        <v>46127.45833333334</v>
+      </c>
+      <c r="M251" t="inlineStr">
+        <is>
           <t>£200,000</t>
         </is>
       </c>
-      <c r="N250" s="1" t="n">
+      <c r="N251" s="1" t="n">
         <v>46064</v>
       </c>
     </row>
@@ -14447,10 +14573,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C2" t="n">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3">
@@ -14473,10 +14599,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C4" t="n">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5">

</xml_diff>